<commit_message>
little progress on project sprint1, added Media as inheritance, compile errors with private access
</commit_message>
<xml_diff>
--- a/Project/Clas Diagram and Backlog/Product Backlog.xlsx
+++ b/Project/Clas Diagram and Backlog/Product Backlog.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="154">
   <si>
     <t xml:space="preserve">Product Name:</t>
   </si>
@@ -445,6 +445,9 @@
   </si>
   <si>
     <t xml:space="preserve">Test get methods in main</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compile Errors with accessing private variables</t>
   </si>
   <si>
     <t xml:space="preserve">Do the same for all other methods and classes</t>
@@ -600,7 +603,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -610,10 +613,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -705,7 +704,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -780,6 +779,78 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
@@ -852,11 +923,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="60921385"/>
-        <c:axId val="79128945"/>
+        <c:axId val="72855111"/>
+        <c:axId val="25023208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="60921385"/>
+        <c:axId val="72855111"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -930,14 +1001,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79128945"/>
+        <c:crossAx val="25023208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79128945"/>
+        <c:axId val="25023208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1018,7 +1089,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60921385"/>
+        <c:crossAx val="72855111"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1046,7 +1117,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1110,6 +1181,100 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
@@ -1194,11 +1359,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="56550409"/>
-        <c:axId val="84241411"/>
+        <c:axId val="34646987"/>
+        <c:axId val="46405646"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="56550409"/>
+        <c:axId val="34646987"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1272,14 +1437,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84241411"/>
+        <c:crossAx val="46405646"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84241411"/>
+        <c:axId val="46405646"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1360,7 +1525,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56550409"/>
+        <c:crossAx val="34646987"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1388,7 +1553,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1452,6 +1617,100 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
@@ -1536,11 +1795,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="55919465"/>
-        <c:axId val="3464796"/>
+        <c:axId val="92250099"/>
+        <c:axId val="55934439"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="55919465"/>
+        <c:axId val="92250099"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1614,14 +1873,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3464796"/>
+        <c:crossAx val="55934439"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="3464796"/>
+        <c:axId val="55934439"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1702,7 +1961,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55919465"/>
+        <c:crossAx val="92250099"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1730,7 +1989,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1794,6 +2053,100 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
@@ -1878,11 +2231,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="7788007"/>
-        <c:axId val="39477808"/>
+        <c:axId val="16974159"/>
+        <c:axId val="2548487"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="7788007"/>
+        <c:axId val="16974159"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1956,14 +2309,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39477808"/>
+        <c:crossAx val="2548487"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39477808"/>
+        <c:axId val="2548487"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2044,7 +2397,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7788007"/>
+        <c:crossAx val="16974159"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2072,7 +2425,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2136,6 +2489,100 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
@@ -2220,11 +2667,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="97105756"/>
-        <c:axId val="11485209"/>
+        <c:axId val="55010570"/>
+        <c:axId val="15112954"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="97105756"/>
+        <c:axId val="55010570"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2298,14 +2745,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11485209"/>
+        <c:crossAx val="15112954"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="11485209"/>
+        <c:axId val="15112954"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2386,7 +2833,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97105756"/>
+        <c:crossAx val="55010570"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2414,7 +2861,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2478,6 +2925,100 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
@@ -2562,11 +3103,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="1866641"/>
-        <c:axId val="15402278"/>
+        <c:axId val="81585118"/>
+        <c:axId val="60130685"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1866641"/>
+        <c:axId val="81585118"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2640,14 +3181,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15402278"/>
+        <c:crossAx val="60130685"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="15402278"/>
+        <c:axId val="60130685"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2728,7 +3269,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1866641"/>
+        <c:crossAx val="81585118"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2767,9 +3308,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>205200</xdr:colOff>
+      <xdr:colOff>204840</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>87120</xdr:rowOff>
+      <xdr:rowOff>86760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2777,8 +3318,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5714640" y="87480"/>
-        <a:ext cx="11759040" cy="2742840"/>
+        <a:off x="5724360" y="87480"/>
+        <a:ext cx="11835000" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2802,9 +3343,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>7560</xdr:colOff>
+      <xdr:colOff>7200</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
+      <xdr:rowOff>37800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2812,8 +3353,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2897280" y="23040"/>
-        <a:ext cx="7502040" cy="2750400"/>
+        <a:off x="2907000" y="23040"/>
+        <a:ext cx="7548840" cy="2750040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2837,9 +3378,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>335160</xdr:colOff>
+      <xdr:colOff>334800</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>22680</xdr:rowOff>
+      <xdr:rowOff>22320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2847,8 +3388,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2459160" y="23040"/>
-        <a:ext cx="5638680" cy="2742840"/>
+        <a:off x="2468880" y="23040"/>
+        <a:ext cx="5638320" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2872,9 +3413,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>335160</xdr:colOff>
+      <xdr:colOff>334800</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>22680</xdr:rowOff>
+      <xdr:rowOff>22320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2882,8 +3423,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2459160" y="23040"/>
-        <a:ext cx="5638680" cy="2742840"/>
+        <a:off x="2468880" y="23040"/>
+        <a:ext cx="5638320" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2907,9 +3448,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>335160</xdr:colOff>
+      <xdr:colOff>334800</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>22680</xdr:rowOff>
+      <xdr:rowOff>22320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2917,8 +3458,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2459160" y="23040"/>
-        <a:ext cx="5638680" cy="2742840"/>
+        <a:off x="2468880" y="23040"/>
+        <a:ext cx="5638320" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2942,9 +3483,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>335160</xdr:colOff>
+      <xdr:colOff>334800</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>22680</xdr:rowOff>
+      <xdr:rowOff>22320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2952,8 +3493,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2459160" y="23040"/>
-        <a:ext cx="5638680" cy="2742840"/>
+        <a:off x="2468880" y="23040"/>
+        <a:ext cx="5638320" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2982,10 +3523,10 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.96356275303644"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.8825910931174"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.5263157894737"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.2064777327935"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.9554655870445"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3146,21 +3687,20 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="3"/>
       <c r="E14" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5"/>
+      <c r="A19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
@@ -3204,7 +3744,7 @@
       <c r="C21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="3" t="n">
+      <c r="D21" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E21" s="1" t="n">
@@ -4036,11 +4576,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2834008097166"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="48.7408906882591"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.4615384615385"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.165991902834"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.5668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -4056,7 +4596,7 @@
       <c r="A2" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="6" t="n">
+      <c r="B2" s="5" t="n">
         <v>43183</v>
       </c>
     </row>
@@ -4064,7 +4604,7 @@
       <c r="A3" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="6" t="n">
+      <c r="B3" s="5" t="n">
         <v>43189</v>
       </c>
     </row>
@@ -4184,7 +4724,7 @@
       <c r="F18" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G18" s="6" t="s">
         <v>126</v>
       </c>
       <c r="H18" s="0" t="s">
@@ -4326,7 +4866,10 @@
         <v>139</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>135</v>
+        <v>126</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4336,23 +4879,23 @@
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>27</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>123</v>
@@ -4361,7 +4904,7 @@
         <v>124</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G29" s="0" t="s">
         <v>135</v>
@@ -4369,7 +4912,7 @@
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>34</v>
@@ -4384,7 +4927,7 @@
         <v>124</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G30" s="0" t="s">
         <v>135</v>
@@ -4392,27 +4935,27 @@
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E33" s="0" t="s">
         <v>124</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G33" s="0" t="s">
         <v>135</v>
@@ -4443,7 +4986,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -4459,7 +5002,7 @@
       <c r="A2" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="6" t="n">
+      <c r="B2" s="5" t="n">
         <v>43192</v>
       </c>
     </row>
@@ -4467,7 +5010,7 @@
       <c r="A3" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="6" t="n">
+      <c r="B3" s="5" t="n">
         <v>43198</v>
       </c>
     </row>
@@ -4594,7 +5137,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -4610,7 +5153,7 @@
       <c r="A2" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="6" t="n">
+      <c r="B2" s="5" t="n">
         <v>43199</v>
       </c>
     </row>
@@ -4618,7 +5161,7 @@
       <c r="A3" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="6" t="n">
+      <c r="B3" s="5" t="n">
         <v>43205</v>
       </c>
     </row>
@@ -4745,7 +5288,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -4761,7 +5304,7 @@
       <c r="A2" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="6" t="n">
+      <c r="B2" s="5" t="n">
         <v>43206</v>
       </c>
     </row>
@@ -4769,7 +5312,7 @@
       <c r="A3" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="6" t="n">
+      <c r="B3" s="5" t="n">
         <v>43212</v>
       </c>
     </row>
@@ -4896,7 +5439,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -4912,7 +5455,7 @@
       <c r="A2" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="6" t="n">
+      <c r="B2" s="5" t="n">
         <v>43213</v>
       </c>
     </row>
@@ -4920,7 +5463,7 @@
       <c r="A3" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="6" t="n">
+      <c r="B3" s="5" t="n">
         <v>43219</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated Sprint1 Backlog chart
</commit_message>
<xml_diff>
--- a/Project/Clas Diagram and Backlog/Product Backlog.xlsx
+++ b/Project/Clas Diagram and Backlog/Product Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="153">
   <si>
     <t xml:space="preserve">Product Name:</t>
   </si>
@@ -405,7 +405,7 @@
     <t xml:space="preserve">Add methods to Media and derived classes</t>
   </si>
   <si>
-    <t xml:space="preserve">S – Started</t>
+    <t xml:space="preserve">C – Completed</t>
   </si>
   <si>
     <t xml:space="preserve">Added get methods only.</t>
@@ -418,9 +418,6 @@
   </si>
   <si>
     <t xml:space="preserve">Write and compile empty Media class</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C – Completed</t>
   </si>
   <si>
     <t xml:space="preserve">Variables and Constructor</t>
@@ -783,9 +780,7 @@
             <c:idx val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="004586">
-                  <a:alpha val="-17698000"/>
-                </a:srgbClr>
+                <a:srgbClr val="004586"/>
               </a:solidFill>
               <a:ln w="6407280">
                 <a:noFill/>
@@ -798,7 +793,7 @@
               <a:solidFill>
                 <a:srgbClr val="ff420e"/>
               </a:solidFill>
-              <a:ln w="6022292400">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -809,7 +804,7 @@
               <a:solidFill>
                 <a:srgbClr val="ffd320"/>
               </a:solidFill>
-              <a:ln w="6035662080">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -818,9 +813,7 @@
             <c:idx val="3"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="579d1c">
-                  <a:alpha val="-1446784704"/>
-                </a:srgbClr>
+                <a:srgbClr val="579d1c"/>
               </a:solidFill>
               <a:ln w="2067066720">
                 <a:noFill/>
@@ -833,7 +826,7 @@
               <a:solidFill>
                 <a:srgbClr val="7e0021"/>
               </a:solidFill>
-              <a:ln w="2972724840">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -842,16 +835,68 @@
             <c:idx val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="83caff">
-                  <a:alpha val="-47148408"/>
-                </a:srgbClr>
+                <a:srgbClr val="83caff"/>
               </a:solidFill>
-              <a:ln w="3109385880">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
           </c:dPt>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -923,11 +968,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="72855111"/>
-        <c:axId val="25023208"/>
+        <c:axId val="63389264"/>
+        <c:axId val="2654840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="72855111"/>
+        <c:axId val="63389264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1001,14 +1046,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25023208"/>
+        <c:crossAx val="2654840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="25023208"/>
+        <c:axId val="2654840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1089,7 +1134,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72855111"/>
+        <c:crossAx val="63389264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1185,9 +1230,7 @@
             <c:idx val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="004586">
-                  <a:alpha val="-17698000"/>
-                </a:srgbClr>
+                <a:srgbClr val="004586"/>
               </a:solidFill>
               <a:ln w="6407280">
                 <a:noFill/>
@@ -1200,7 +1243,7 @@
               <a:solidFill>
                 <a:srgbClr val="ff420e"/>
               </a:solidFill>
-              <a:ln w="6022292400">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -1211,7 +1254,7 @@
               <a:solidFill>
                 <a:srgbClr val="ffd320"/>
               </a:solidFill>
-              <a:ln w="6035662080">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -1220,9 +1263,7 @@
             <c:idx val="3"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="579d1c">
-                  <a:alpha val="-1446784704"/>
-                </a:srgbClr>
+                <a:srgbClr val="579d1c"/>
               </a:solidFill>
               <a:ln w="2067066720">
                 <a:noFill/>
@@ -1235,7 +1276,7 @@
               <a:solidFill>
                 <a:srgbClr val="7e0021"/>
               </a:solidFill>
-              <a:ln w="2972724840">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -1244,11 +1285,9 @@
             <c:idx val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="83caff">
-                  <a:alpha val="-47148408"/>
-                </a:srgbClr>
+                <a:srgbClr val="83caff"/>
               </a:solidFill>
-              <a:ln w="3109385880">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -1270,12 +1309,84 @@
               <a:solidFill>
                 <a:srgbClr val="aecf00"/>
               </a:solidFill>
-              <a:ln w="4124252160">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
           </c:dPt>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -1326,10 +1437,10 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>5</c:v>
@@ -1341,10 +1452,10 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1359,11 +1470,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="34646987"/>
-        <c:axId val="46405646"/>
+        <c:axId val="81912389"/>
+        <c:axId val="76323020"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="34646987"/>
+        <c:axId val="81912389"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1437,14 +1548,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46405646"/>
+        <c:crossAx val="76323020"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46405646"/>
+        <c:axId val="76323020"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1525,7 +1636,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34646987"/>
+        <c:crossAx val="81912389"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1621,9 +1732,7 @@
             <c:idx val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="004586">
-                  <a:alpha val="-17698000"/>
-                </a:srgbClr>
+                <a:srgbClr val="004586"/>
               </a:solidFill>
               <a:ln w="6407280">
                 <a:noFill/>
@@ -1636,7 +1745,7 @@
               <a:solidFill>
                 <a:srgbClr val="ff420e"/>
               </a:solidFill>
-              <a:ln w="6022292400">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -1647,7 +1756,7 @@
               <a:solidFill>
                 <a:srgbClr val="ffd320"/>
               </a:solidFill>
-              <a:ln w="6035662080">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -1656,9 +1765,7 @@
             <c:idx val="3"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="579d1c">
-                  <a:alpha val="-1446784704"/>
-                </a:srgbClr>
+                <a:srgbClr val="579d1c"/>
               </a:solidFill>
               <a:ln w="2067066720">
                 <a:noFill/>
@@ -1671,7 +1778,7 @@
               <a:solidFill>
                 <a:srgbClr val="7e0021"/>
               </a:solidFill>
-              <a:ln w="2972724840">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -1680,11 +1787,9 @@
             <c:idx val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="83caff">
-                  <a:alpha val="-47148408"/>
-                </a:srgbClr>
+                <a:srgbClr val="83caff"/>
               </a:solidFill>
-              <a:ln w="3109385880">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -1706,12 +1811,84 @@
               <a:solidFill>
                 <a:srgbClr val="aecf00"/>
               </a:solidFill>
-              <a:ln w="4124252160">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
           </c:dPt>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -1795,11 +1972,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="92250099"/>
-        <c:axId val="55934439"/>
+        <c:axId val="47268638"/>
+        <c:axId val="22501096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="92250099"/>
+        <c:axId val="47268638"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1873,14 +2050,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55934439"/>
+        <c:crossAx val="22501096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="55934439"/>
+        <c:axId val="22501096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1961,7 +2138,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92250099"/>
+        <c:crossAx val="47268638"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2057,9 +2234,7 @@
             <c:idx val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="004586">
-                  <a:alpha val="-17698000"/>
-                </a:srgbClr>
+                <a:srgbClr val="004586"/>
               </a:solidFill>
               <a:ln w="6407280">
                 <a:noFill/>
@@ -2072,7 +2247,7 @@
               <a:solidFill>
                 <a:srgbClr val="ff420e"/>
               </a:solidFill>
-              <a:ln w="6022292400">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -2083,7 +2258,7 @@
               <a:solidFill>
                 <a:srgbClr val="ffd320"/>
               </a:solidFill>
-              <a:ln w="6035662080">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -2092,9 +2267,7 @@
             <c:idx val="3"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="579d1c">
-                  <a:alpha val="-1446784704"/>
-                </a:srgbClr>
+                <a:srgbClr val="579d1c"/>
               </a:solidFill>
               <a:ln w="2067066720">
                 <a:noFill/>
@@ -2107,7 +2280,7 @@
               <a:solidFill>
                 <a:srgbClr val="7e0021"/>
               </a:solidFill>
-              <a:ln w="2972724840">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -2116,11 +2289,9 @@
             <c:idx val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="83caff">
-                  <a:alpha val="-47148408"/>
-                </a:srgbClr>
+                <a:srgbClr val="83caff"/>
               </a:solidFill>
-              <a:ln w="3109385880">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -2142,12 +2313,84 @@
               <a:solidFill>
                 <a:srgbClr val="aecf00"/>
               </a:solidFill>
-              <a:ln w="4124252160">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
           </c:dPt>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -2231,11 +2474,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="16974159"/>
-        <c:axId val="2548487"/>
+        <c:axId val="39275903"/>
+        <c:axId val="11841848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="16974159"/>
+        <c:axId val="39275903"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2309,14 +2552,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2548487"/>
+        <c:crossAx val="11841848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2548487"/>
+        <c:axId val="11841848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2397,7 +2640,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16974159"/>
+        <c:crossAx val="39275903"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2493,9 +2736,7 @@
             <c:idx val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="004586">
-                  <a:alpha val="-17698000"/>
-                </a:srgbClr>
+                <a:srgbClr val="004586"/>
               </a:solidFill>
               <a:ln w="6407280">
                 <a:noFill/>
@@ -2508,7 +2749,7 @@
               <a:solidFill>
                 <a:srgbClr val="ff420e"/>
               </a:solidFill>
-              <a:ln w="6022292400">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -2519,7 +2760,7 @@
               <a:solidFill>
                 <a:srgbClr val="ffd320"/>
               </a:solidFill>
-              <a:ln w="6035662080">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -2528,9 +2769,7 @@
             <c:idx val="3"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="579d1c">
-                  <a:alpha val="-1446784704"/>
-                </a:srgbClr>
+                <a:srgbClr val="579d1c"/>
               </a:solidFill>
               <a:ln w="2067066720">
                 <a:noFill/>
@@ -2543,7 +2782,7 @@
               <a:solidFill>
                 <a:srgbClr val="7e0021"/>
               </a:solidFill>
-              <a:ln w="2972724840">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -2552,11 +2791,9 @@
             <c:idx val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="83caff">
-                  <a:alpha val="-47148408"/>
-                </a:srgbClr>
+                <a:srgbClr val="83caff"/>
               </a:solidFill>
-              <a:ln w="3109385880">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -2578,12 +2815,84 @@
               <a:solidFill>
                 <a:srgbClr val="aecf00"/>
               </a:solidFill>
-              <a:ln w="4124252160">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
           </c:dPt>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -2667,11 +2976,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="55010570"/>
-        <c:axId val="15112954"/>
+        <c:axId val="47814892"/>
+        <c:axId val="8439301"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="55010570"/>
+        <c:axId val="47814892"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2745,14 +3054,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15112954"/>
+        <c:crossAx val="8439301"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="15112954"/>
+        <c:axId val="8439301"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2833,7 +3142,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55010570"/>
+        <c:crossAx val="47814892"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2929,9 +3238,7 @@
             <c:idx val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="004586">
-                  <a:alpha val="-17698000"/>
-                </a:srgbClr>
+                <a:srgbClr val="004586"/>
               </a:solidFill>
               <a:ln w="6407280">
                 <a:noFill/>
@@ -2944,7 +3251,7 @@
               <a:solidFill>
                 <a:srgbClr val="ff420e"/>
               </a:solidFill>
-              <a:ln w="6022292400">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -2955,7 +3262,7 @@
               <a:solidFill>
                 <a:srgbClr val="ffd320"/>
               </a:solidFill>
-              <a:ln w="6035662080">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -2964,9 +3271,7 @@
             <c:idx val="3"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="579d1c">
-                  <a:alpha val="-1446784704"/>
-                </a:srgbClr>
+                <a:srgbClr val="579d1c"/>
               </a:solidFill>
               <a:ln w="2067066720">
                 <a:noFill/>
@@ -2979,7 +3284,7 @@
               <a:solidFill>
                 <a:srgbClr val="7e0021"/>
               </a:solidFill>
-              <a:ln w="2972724840">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -2988,11 +3293,9 @@
             <c:idx val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="83caff">
-                  <a:alpha val="-47148408"/>
-                </a:srgbClr>
+                <a:srgbClr val="83caff"/>
               </a:solidFill>
-              <a:ln w="3109385880">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -3014,12 +3317,84 @@
               <a:solidFill>
                 <a:srgbClr val="aecf00"/>
               </a:solidFill>
-              <a:ln w="4124252160">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
           </c:dPt>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -3103,11 +3478,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="81585118"/>
-        <c:axId val="60130685"/>
+        <c:axId val="60943841"/>
+        <c:axId val="14942994"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="81585118"/>
+        <c:axId val="60943841"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3181,14 +3556,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60130685"/>
+        <c:crossAx val="14942994"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60130685"/>
+        <c:axId val="14942994"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3269,7 +3644,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81585118"/>
+        <c:crossAx val="60943841"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3308,9 +3683,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>204840</xdr:colOff>
+      <xdr:colOff>204480</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>86760</xdr:rowOff>
+      <xdr:rowOff>86400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3318,8 +3693,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5724360" y="87480"/>
-        <a:ext cx="11835000" cy="2742480"/>
+        <a:off x="5733720" y="87480"/>
+        <a:ext cx="11910960" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3343,9 +3718,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>7200</xdr:colOff>
+      <xdr:colOff>6840</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>37800</xdr:rowOff>
+      <xdr:rowOff>45000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3353,8 +3728,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2907000" y="23040"/>
-        <a:ext cx="7548840" cy="2750040"/>
+        <a:off x="2916360" y="23040"/>
+        <a:ext cx="7587000" cy="2749680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3378,9 +3753,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>334800</xdr:colOff>
+      <xdr:colOff>334440</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>22320</xdr:rowOff>
+      <xdr:rowOff>21960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3388,8 +3763,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2468880" y="23040"/>
-        <a:ext cx="5638320" cy="2742480"/>
+        <a:off x="2478240" y="23040"/>
+        <a:ext cx="5637960" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3413,9 +3788,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>334800</xdr:colOff>
+      <xdr:colOff>334440</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>22320</xdr:rowOff>
+      <xdr:rowOff>21960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3423,8 +3798,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2468880" y="23040"/>
-        <a:ext cx="5638320" cy="2742480"/>
+        <a:off x="2478240" y="23040"/>
+        <a:ext cx="5637960" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3448,9 +3823,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>334800</xdr:colOff>
+      <xdr:colOff>334440</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>22320</xdr:rowOff>
+      <xdr:rowOff>21960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3458,8 +3833,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2468880" y="23040"/>
-        <a:ext cx="5638320" cy="2742480"/>
+        <a:off x="2478240" y="23040"/>
+        <a:ext cx="5637960" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3483,9 +3858,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>334800</xdr:colOff>
+      <xdr:colOff>334440</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>22320</xdr:rowOff>
+      <xdr:rowOff>21960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3493,8 +3868,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2468880" y="23040"/>
-        <a:ext cx="5638320" cy="2742480"/>
+        <a:off x="2478240" y="23040"/>
+        <a:ext cx="5637960" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3514,8 +3889,8 @@
   </sheetPr>
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3523,10 +3898,10 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.0688259109312"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.2064777327935"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.9554655870445"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.5263157894737"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.3805668016194"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3809,7 +4184,9 @@
       <c r="D23" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E23" s="1"/>
+      <c r="E23" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="F23" s="0" t="s">
         <v>29</v>
       </c>
@@ -3838,7 +4215,9 @@
       <c r="D24" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E24" s="1"/>
+      <c r="E24" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="F24" s="0" t="s">
         <v>39</v>
       </c>
@@ -4570,17 +4949,17 @@
   </sheetPr>
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.165991902834"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.4898785425101"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.6761133603239"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -4622,7 +5001,8 @@
         <v>111</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>5</v>
+        <f aca="false">B5</f>
+        <v>8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4631,7 +5011,7 @@
       </c>
       <c r="B7" s="1" t="n">
         <f aca="false">B6</f>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4639,7 +5019,6 @@
         <v>113</v>
       </c>
       <c r="B8" s="1" t="n">
-        <f aca="false">B7</f>
         <v>5</v>
       </c>
     </row>
@@ -4652,7 +5031,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>115</v>
       </c>
@@ -4666,8 +5045,7 @@
         <v>116</v>
       </c>
       <c r="B11" s="1" t="n">
-        <f aca="false">B10</f>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4676,7 +5054,7 @@
       </c>
       <c r="B12" s="1" t="n">
         <f aca="false">B11</f>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4751,7 +5129,7 @@
         <v>130</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4771,10 +5149,10 @@
         <v>124</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4788,16 +5166,16 @@
         <v>128</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>124</v>
       </c>
       <c r="F21" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="G21" s="0" t="s">
         <v>134</v>
-      </c>
-      <c r="G21" s="0" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4811,16 +5189,16 @@
         <v>128</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>124</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4840,13 +5218,13 @@
         <v>124</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>7</v>
       </c>
@@ -4857,19 +5235,19 @@
         <v>128</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>124</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G24" s="0" t="s">
         <v>126</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4879,23 +5257,23 @@
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>27</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>123</v>
@@ -4904,15 +5282,15 @@
         <v>124</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>34</v>
@@ -4927,38 +5305,38 @@
         <v>124</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B33" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="C33" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="D33" s="0" t="s">
         <v>151</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>152</v>
       </c>
       <c r="E33" s="0" t="s">
         <v>124</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -4986,7 +5364,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -5137,7 +5515,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -5288,7 +5666,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -5439,7 +5817,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
a little progress on operator overloading <<, compiled and working correctly
</commit_message>
<xml_diff>
--- a/Project/Clas Diagram and Backlog/Product Backlog.xlsx
+++ b/Project/Clas Diagram and Backlog/Product Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="154">
   <si>
     <t xml:space="preserve">Product Name:</t>
   </si>
@@ -429,37 +429,40 @@
     <t xml:space="preserve">Operator Overload &lt;&lt;</t>
   </si>
   <si>
+    <t xml:space="preserve">S – Started</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Constructor and &lt;&lt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add Get Methods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test get methods in main</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compile Errors with accessing private variables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do the same for all other methods and classes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should detail out all tasks done for completing this project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wrap Up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update UML to match new methods if changed</t>
+  </si>
+  <si>
     <t xml:space="preserve">NS - Not Started</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Constructor and &lt;&lt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add Get Methods</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test get methods in main</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compile Errors with accessing private variables</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do the same for all other methods and classes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Should detail out all tasks done for completing this project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wrap Up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Update UML to match new methods if changed</t>
   </si>
   <si>
     <t xml:space="preserve">N + 1</t>
@@ -701,7 +704,1513 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>Sprint Burn Down Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="5b9bd5"/>
+            </a:solidFill>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="5b9bd5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 3'!$A$5:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Total Tasks</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day 1 Left</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day 2 Left</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Day 3 Left</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Day 4 Left</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Day 5 Left</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Day 6 Left</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Day 7 Left</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 3'!$B$5:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="60979869"/>
+        <c:axId val="86794746"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="60979869"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Day</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="d9d9d9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="86794746"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="86794746"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Tasks Remaining</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="60979869"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>Sprint Burn Down Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="5b9bd5"/>
+            </a:solidFill>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="5b9bd5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 4'!$A$5:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Total Tasks</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day 1 Left</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day 2 Left</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Day 3 Left</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Day 4 Left</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Day 5 Left</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Day 6 Left</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Day 7 Left</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 4'!$B$5:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="4370797"/>
+        <c:axId val="75019675"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="4370797"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Day</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="d9d9d9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="75019675"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="75019675"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Tasks Remaining</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="4370797"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>Sprint Burn Down Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="5b9bd5"/>
+            </a:solidFill>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="5b9bd5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 5'!$A$5:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Total Tasks</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day 1 Left</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day 2 Left</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Day 3 Left</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Day 4 Left</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Day 5 Left</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Day 6 Left</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Day 7 Left</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 5'!$B$5:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="40482656"/>
+        <c:axId val="6160366"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="40482656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Day</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="d9d9d9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="6160366"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="6160366"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Tasks Remaining</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="40482656"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -968,11 +2477,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="63389264"/>
-        <c:axId val="2654840"/>
+        <c:axId val="61489655"/>
+        <c:axId val="55911990"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63389264"/>
+        <c:axId val="61489655"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1046,14 +2555,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2654840"/>
+        <c:crossAx val="55911990"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2654840"/>
+        <c:axId val="55911990"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1134,7 +2643,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63389264"/>
+        <c:crossAx val="61489655"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1162,7 +2671,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1470,11 +2979,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="81912389"/>
-        <c:axId val="76323020"/>
+        <c:axId val="17671980"/>
+        <c:axId val="98710399"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="81912389"/>
+        <c:axId val="17671980"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1548,14 +3057,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76323020"/>
+        <c:crossAx val="98710399"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76323020"/>
+        <c:axId val="98710399"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1636,7 +3145,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81912389"/>
+        <c:crossAx val="17671980"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1664,7 +3173,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1972,11 +3481,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="47268638"/>
-        <c:axId val="22501096"/>
+        <c:axId val="79699088"/>
+        <c:axId val="62213908"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="47268638"/>
+        <c:axId val="79699088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2050,14 +3559,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22501096"/>
+        <c:crossAx val="62213908"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="22501096"/>
+        <c:axId val="62213908"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2138,1513 +3647,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47268638"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>Sprint Burn Down Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="5b9bd5"/>
-            </a:solidFill>
-            <a:ln w="28440">
-              <a:solidFill>
-                <a:srgbClr val="5b9bd5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="6407280">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="2067066720">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="6"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="314004"/>
-              </a:solidFill>
-              <a:ln w="1161954720">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="7"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="aecf00"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="6"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="7"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Sprint 3'!$A$5:$A$12</c:f>
-              <c:strCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>Total Tasks</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Day 1 Left</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Day 2 Left</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Day 3 Left</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Day 4 Left</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Day 5 Left</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Day 6 Left</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Day 7 Left</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sprint 3'!$B$5:$B$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="39275903"/>
-        <c:axId val="11841848"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="39275903"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Day</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="11841848"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="11841848"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Tasks Remaining</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="39275903"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>Sprint Burn Down Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="5b9bd5"/>
-            </a:solidFill>
-            <a:ln w="28440">
-              <a:solidFill>
-                <a:srgbClr val="5b9bd5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="6407280">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="2067066720">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="6"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="314004"/>
-              </a:solidFill>
-              <a:ln w="1161954720">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="7"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="aecf00"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="6"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="7"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Sprint 4'!$A$5:$A$12</c:f>
-              <c:strCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>Total Tasks</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Day 1 Left</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Day 2 Left</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Day 3 Left</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Day 4 Left</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Day 5 Left</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Day 6 Left</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Day 7 Left</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sprint 4'!$B$5:$B$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="47814892"/>
-        <c:axId val="8439301"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="47814892"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Day</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="8439301"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="8439301"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Tasks Remaining</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="47814892"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>Sprint Burn Down Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="5b9bd5"/>
-            </a:solidFill>
-            <a:ln w="28440">
-              <a:solidFill>
-                <a:srgbClr val="5b9bd5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="6407280">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="2067066720">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="6"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="314004"/>
-              </a:solidFill>
-              <a:ln w="1161954720">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="7"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="aecf00"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="6"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="7"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Sprint 5'!$A$5:$A$12</c:f>
-              <c:strCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>Total Tasks</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Day 1 Left</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Day 2 Left</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Day 3 Left</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Day 4 Left</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Day 5 Left</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Day 6 Left</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Day 7 Left</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sprint 5'!$B$5:$B$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="60943841"/>
-        <c:axId val="14942994"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="60943841"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Day</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="14942994"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="14942994"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Tasks Remaining</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="60943841"/>
+        <c:crossAx val="79699088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3683,9 +3686,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>204480</xdr:colOff>
+      <xdr:colOff>204120</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>86400</xdr:rowOff>
+      <xdr:rowOff>86040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3693,8 +3696,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5733720" y="87480"/>
-        <a:ext cx="11910960" cy="2742120"/>
+        <a:off x="5743440" y="87480"/>
+        <a:ext cx="11976840" cy="2741760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3718,9 +3721,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>6840</xdr:colOff>
+      <xdr:colOff>6480</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>45000</xdr:rowOff>
+      <xdr:rowOff>44640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3729,7 +3732,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2916360" y="23040"/>
-        <a:ext cx="7587000" cy="2749680"/>
+        <a:ext cx="7624440" cy="2749320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3753,9 +3756,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>334440</xdr:colOff>
+      <xdr:colOff>334080</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>21960</xdr:rowOff>
+      <xdr:rowOff>21600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3764,7 +3767,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5637960" cy="2742120"/>
+        <a:ext cx="5637600" cy="2741760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3788,9 +3791,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>334440</xdr:colOff>
+      <xdr:colOff>334080</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>21960</xdr:rowOff>
+      <xdr:rowOff>21600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3799,7 +3802,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5637960" cy="2742120"/>
+        <a:ext cx="5637600" cy="2741760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3823,9 +3826,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>334440</xdr:colOff>
+      <xdr:colOff>334080</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>21960</xdr:rowOff>
+      <xdr:rowOff>21600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3834,7 +3837,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5637960" cy="2742120"/>
+        <a:ext cx="5637600" cy="2741760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3858,9 +3861,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>334440</xdr:colOff>
+      <xdr:colOff>334080</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>21960</xdr:rowOff>
+      <xdr:rowOff>21600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3869,7 +3872,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5637960" cy="2742120"/>
+        <a:ext cx="5637600" cy="2741760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3889,7 +3892,7 @@
   </sheetPr>
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -3898,10 +3901,10 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.1781376518219"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.5263157894737"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.3805668016194"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.8502024291498"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.7044534412956"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -4155,7 +4158,9 @@
       <c r="D22" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E22" s="1"/>
+      <c r="E22" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="F22" s="0" t="s">
         <v>29</v>
       </c>
@@ -4949,8 +4954,8 @@
   </sheetPr>
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4958,8 +4963,8 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.4898785425101"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.8097165991903"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.7813765182186"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -5285,12 +5290,12 @@
         <v>144</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>34</v>
@@ -5305,7 +5310,7 @@
         <v>124</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G30" s="0" t="s">
         <v>126</v>
@@ -5313,30 +5318,30 @@
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E33" s="0" t="s">
         <v>124</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated UML and updated outputs
</commit_message>
<xml_diff>
--- a/Project/Clas Diagram and Backlog/Product Backlog.xlsx
+++ b/Project/Clas Diagram and Backlog/Product Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="155">
   <si>
     <t xml:space="preserve">Product Name:</t>
   </si>
@@ -399,94 +399,97 @@
     <t xml:space="preserve">UML</t>
   </si>
   <si>
+    <t xml:space="preserve">AD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add methods to Media and derived classes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C – Completed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added get methods only.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Media</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Write and compile empty Media class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variables and Constructor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operator Overload &lt;&lt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Constructor and &lt;&lt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add Get Methods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test get methods in main</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compile Errors with accessing private variables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do the same for all other methods and classes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should detail out all tasks done for completing this project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wrap Up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update UML to match new methods if changed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N + 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add methods to Bundle and derived classes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S – Started</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Follow Same pattern used in Media for Bundle and all other classes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wrap_Up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delivery</t>
+  </si>
+  <si>
     <t xml:space="preserve">Initials Here</t>
   </si>
   <si>
-    <t xml:space="preserve">Add methods to Media and derived classes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C – Completed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Added get methods only.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Media</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Write and compile empty Media class</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Variables and Constructor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Code </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operator Overload &lt;&lt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S – Started</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Constructor and &lt;&lt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add Get Methods</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test get methods in main</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compile Errors with accessing private variables</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do the same for all other methods and classes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Should detail out all tasks done for completing this project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wrap Up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Update UML to match new methods if changed</t>
+    <t xml:space="preserve">Zip up and deliver sprint #1 (UML, Code, and spreadsheet)</t>
   </si>
   <si>
     <t xml:space="preserve">NS - Not Started</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N + 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add methods to Bundle and derived classes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Follow Same pattern used in Media for Bundle and all other classes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Demo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wrap_Up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delivery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zip up and deliver sprint #1 (UML, Code, and spreadsheet)</t>
   </si>
 </sst>
 </file>
@@ -704,7 +707,1472 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>Product Backlog Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Product Backlog'!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Left</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="5b9bd5"/>
+            </a:solidFill>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="5b9bd5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Product Backlog'!$A$8:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sprint 3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sprint 4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sprint 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Product Backlog'!$B$8:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="91922495"/>
+        <c:axId val="8740667"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="91922495"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Sprint Number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="d9d9d9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="8740667"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="8740667"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Features Left at End of Sprint</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="91922495"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>Sprint Burn Down Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="5b9bd5"/>
+            </a:solidFill>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="5b9bd5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 1'!$A$5:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Total Tasks</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day 1 Left</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day 2 Left</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Day 3 Left</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Day 4 Left</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Day 5 Left</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Day 6 Left</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Day 7 Left</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 1'!$B$5:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="29351604"/>
+        <c:axId val="85432465"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="29351604"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Day</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="d9d9d9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="85432465"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="85432465"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Tasks Remaining</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="29351604"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>Sprint Burn Down Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="5b9bd5"/>
+            </a:solidFill>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="5b9bd5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 2'!$A$5:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Total Tasks</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day 1 Left</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day 2 Left</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Day 3 Left</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Day 4 Left</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Day 5 Left</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Day 6 Left</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Day 7 Left</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 2'!$B$5:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="20120087"/>
+        <c:axId val="31096958"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="20120087"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Day</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="d9d9d9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="31096958"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="31096958"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Tasks Remaining</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="20120087"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1012,11 +2480,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="60979869"/>
-        <c:axId val="86794746"/>
+        <c:axId val="3497110"/>
+        <c:axId val="56760953"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="60979869"/>
+        <c:axId val="3497110"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1090,14 +2558,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86794746"/>
+        <c:crossAx val="56760953"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86794746"/>
+        <c:axId val="56760953"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1178,7 +2646,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60979869"/>
+        <c:crossAx val="3497110"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1206,7 +2674,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1514,11 +2982,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="4370797"/>
-        <c:axId val="75019675"/>
+        <c:axId val="37369685"/>
+        <c:axId val="23368999"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="4370797"/>
+        <c:axId val="37369685"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1592,14 +3060,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75019675"/>
+        <c:crossAx val="23368999"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75019675"/>
+        <c:axId val="23368999"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1680,7 +3148,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4370797"/>
+        <c:crossAx val="37369685"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1708,7 +3176,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2016,11 +3484,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="40482656"/>
-        <c:axId val="6160366"/>
+        <c:axId val="55755600"/>
+        <c:axId val="62319949"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="40482656"/>
+        <c:axId val="55755600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2094,14 +3562,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6160366"/>
+        <c:crossAx val="62319949"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="6160366"/>
+        <c:axId val="62319949"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2182,1472 +3650,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40482656"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>Product Backlog Burn Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Product Backlog'!$B$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Left</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="5b9bd5"/>
-            </a:solidFill>
-            <a:ln w="28440">
-              <a:solidFill>
-                <a:srgbClr val="5b9bd5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="6407280">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="2067066720">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Product Backlog'!$A$8:$A$13</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Start</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Sprint 1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Sprint 2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Sprint 3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sprint 4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Sprint 5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Product Backlog'!$B$8:$B$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>27</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="61489655"/>
-        <c:axId val="55911990"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="61489655"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Sprint Number</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="55911990"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="55911990"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Features Left at End of Sprint</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="61489655"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>Sprint Burn Down Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="5b9bd5"/>
-            </a:solidFill>
-            <a:ln w="28440">
-              <a:solidFill>
-                <a:srgbClr val="5b9bd5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="6407280">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="2067066720">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="6"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="314004"/>
-              </a:solidFill>
-              <a:ln w="1161954720">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="7"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="aecf00"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="6"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="7"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Sprint 1'!$A$5:$A$12</c:f>
-              <c:strCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>Total Tasks</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Day 1 Left</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Day 2 Left</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Day 3 Left</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Day 4 Left</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Day 5 Left</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Day 6 Left</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Day 7 Left</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sprint 1'!$B$5:$B$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="17671980"/>
-        <c:axId val="98710399"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="17671980"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Day</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="98710399"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="98710399"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Tasks Remaining</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="17671980"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>Sprint Burn Down Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="5b9bd5"/>
-            </a:solidFill>
-            <a:ln w="28440">
-              <a:solidFill>
-                <a:srgbClr val="5b9bd5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="6407280">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="2067066720">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="6"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="314004"/>
-              </a:solidFill>
-              <a:ln w="1161954720">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="7"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="aecf00"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="6"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="7"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Sprint 2'!$A$5:$A$12</c:f>
-              <c:strCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>Total Tasks</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Day 1 Left</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Day 2 Left</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Day 3 Left</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Day 4 Left</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Day 5 Left</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Day 6 Left</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Day 7 Left</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sprint 2'!$B$5:$B$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="79699088"/>
-        <c:axId val="62213908"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="79699088"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Day</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="62213908"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="62213908"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Tasks Remaining</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="79699088"/>
+        <c:crossAx val="55755600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3686,9 +3689,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>204120</xdr:colOff>
+      <xdr:colOff>203760</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>86040</xdr:rowOff>
+      <xdr:rowOff>85680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3696,8 +3699,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5743440" y="87480"/>
-        <a:ext cx="11976840" cy="2741760"/>
+        <a:off x="5752800" y="87480"/>
+        <a:ext cx="12043440" cy="2741400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3721,9 +3724,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>6480</xdr:colOff>
+      <xdr:colOff>6120</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>44640</xdr:rowOff>
+      <xdr:rowOff>44280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3732,7 +3735,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2916360" y="23040"/>
-        <a:ext cx="7624440" cy="2749320"/>
+        <a:ext cx="7671960" cy="2748960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3756,9 +3759,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>334080</xdr:colOff>
+      <xdr:colOff>333720</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>21600</xdr:rowOff>
+      <xdr:rowOff>21240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3767,7 +3770,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5637600" cy="2741760"/>
+        <a:ext cx="5637240" cy="2741400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3791,9 +3794,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>334080</xdr:colOff>
+      <xdr:colOff>333720</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>21600</xdr:rowOff>
+      <xdr:rowOff>21240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3802,7 +3805,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5637600" cy="2741760"/>
+        <a:ext cx="5637240" cy="2741400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3826,9 +3829,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>334080</xdr:colOff>
+      <xdr:colOff>333720</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>21600</xdr:rowOff>
+      <xdr:rowOff>21240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3837,7 +3840,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5637600" cy="2741760"/>
+        <a:ext cx="5637240" cy="2741400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3861,9 +3864,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>334080</xdr:colOff>
+      <xdr:colOff>333720</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>21600</xdr:rowOff>
+      <xdr:rowOff>21240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3872,7 +3875,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5637600" cy="2741760"/>
+        <a:ext cx="5637240" cy="2741400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3892,8 +3895,8 @@
   </sheetPr>
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3901,10 +3904,10 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.8502024291498"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.7044534412956"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.17004048583"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.0242914979757"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -4955,7 +4958,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4963,8 +4966,8 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.8097165991903"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.2388663967611"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.8906882591093"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -5050,7 +5053,7 @@
         <v>116</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5058,8 +5061,7 @@
         <v>117</v>
       </c>
       <c r="B12" s="1" t="n">
-        <f aca="false">B11</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5114,7 +5116,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>2</v>
       </c>
@@ -5137,7 +5139,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>3</v>
       </c>
@@ -5160,7 +5162,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>4</v>
       </c>
@@ -5180,10 +5182,10 @@
         <v>133</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>5</v>
       </c>
@@ -5194,19 +5196,19 @@
         <v>128</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>124</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>6</v>
       </c>
@@ -5223,7 +5225,7 @@
         <v>124</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G23" s="0" t="s">
         <v>126</v>
@@ -5240,19 +5242,19 @@
         <v>128</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>124</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G24" s="0" t="s">
         <v>126</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5262,23 +5264,23 @@
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>142</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>27</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>123</v>
@@ -5287,15 +5289,15 @@
         <v>124</v>
       </c>
       <c r="F29" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
         <v>144</v>
-      </c>
-      <c r="G29" s="0" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>146</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>34</v>
@@ -5310,38 +5312,38 @@
         <v>124</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B33" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="C33" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="D33" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="E33" s="0" t="s">
         <v>152</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>124</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>153</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated files for and7697_sprint1 for submission
</commit_message>
<xml_diff>
--- a/Project/Clas Diagram and Backlog/Product Backlog.xlsx
+++ b/Project/Clas Diagram and Backlog/Product Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="152">
   <si>
     <t xml:space="preserve">Product Name:</t>
   </si>
@@ -441,9 +441,6 @@
     <t xml:space="preserve">Test get methods in main</t>
   </si>
   <si>
-    <t xml:space="preserve">Compile Errors with accessing private variables</t>
-  </si>
-  <si>
     <t xml:space="preserve">Do the same for all other methods and classes</t>
   </si>
   <si>
@@ -465,9 +462,6 @@
     <t xml:space="preserve">Add methods to Bundle and derived classes</t>
   </si>
   <si>
-    <t xml:space="preserve">S – Started</t>
-  </si>
-  <si>
     <t xml:space="preserve">Follow Same pattern used in Media for Bundle and all other classes</t>
   </si>
   <si>
@@ -487,9 +481,6 @@
   </si>
   <si>
     <t xml:space="preserve">Zip up and deliver sprint #1 (UML, Code, and spreadsheet)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NS - Not Started</t>
   </si>
 </sst>
 </file>
@@ -974,11 +965,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="91922495"/>
-        <c:axId val="8740667"/>
+        <c:axId val="50193812"/>
+        <c:axId val="15727160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="91922495"/>
+        <c:axId val="50193812"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1052,14 +1043,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8740667"/>
+        <c:crossAx val="15727160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="8740667"/>
+        <c:axId val="15727160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1140,7 +1131,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91922495"/>
+        <c:crossAx val="50193812"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1476,11 +1467,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="29351604"/>
-        <c:axId val="85432465"/>
+        <c:axId val="28544889"/>
+        <c:axId val="41106859"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="29351604"/>
+        <c:axId val="28544889"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1554,14 +1545,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85432465"/>
+        <c:crossAx val="41106859"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85432465"/>
+        <c:axId val="41106859"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1642,7 +1633,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29351604"/>
+        <c:crossAx val="28544889"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1978,11 +1969,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="20120087"/>
-        <c:axId val="31096958"/>
+        <c:axId val="71032889"/>
+        <c:axId val="16890469"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="20120087"/>
+        <c:axId val="71032889"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2056,14 +2047,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31096958"/>
+        <c:crossAx val="16890469"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="31096958"/>
+        <c:axId val="16890469"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2144,7 +2135,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20120087"/>
+        <c:crossAx val="71032889"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2480,11 +2471,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="3497110"/>
-        <c:axId val="56760953"/>
+        <c:axId val="49081331"/>
+        <c:axId val="4704043"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="3497110"/>
+        <c:axId val="49081331"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2558,14 +2549,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56760953"/>
+        <c:crossAx val="4704043"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="56760953"/>
+        <c:axId val="4704043"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2646,7 +2637,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3497110"/>
+        <c:crossAx val="49081331"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2982,11 +2973,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="37369685"/>
-        <c:axId val="23368999"/>
+        <c:axId val="8971600"/>
+        <c:axId val="8319402"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="37369685"/>
+        <c:axId val="8971600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3060,14 +3051,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23368999"/>
+        <c:crossAx val="8319402"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="23368999"/>
+        <c:axId val="8319402"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3148,7 +3139,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37369685"/>
+        <c:crossAx val="8971600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3484,11 +3475,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="55755600"/>
-        <c:axId val="62319949"/>
+        <c:axId val="67016042"/>
+        <c:axId val="25181228"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="55755600"/>
+        <c:axId val="67016042"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3562,14 +3553,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62319949"/>
+        <c:crossAx val="25181228"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62319949"/>
+        <c:axId val="25181228"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3650,7 +3641,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55755600"/>
+        <c:crossAx val="67016042"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3689,9 +3680,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>203760</xdr:colOff>
+      <xdr:colOff>203400</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>85680</xdr:rowOff>
+      <xdr:rowOff>85320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3699,8 +3690,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5752800" y="87480"/>
-        <a:ext cx="12043440" cy="2741400"/>
+        <a:off x="5762520" y="87480"/>
+        <a:ext cx="12109680" cy="2741040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3724,9 +3715,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>6120</xdr:colOff>
+      <xdr:colOff>5760</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>44280</xdr:rowOff>
+      <xdr:rowOff>43920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3735,7 +3726,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2916360" y="23040"/>
-        <a:ext cx="7671960" cy="2748960"/>
+        <a:ext cx="7719120" cy="2748600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3759,9 +3750,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>333720</xdr:colOff>
+      <xdr:colOff>333360</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>21240</xdr:rowOff>
+      <xdr:rowOff>20880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3770,7 +3761,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5637240" cy="2741400"/>
+        <a:ext cx="5636880" cy="2741040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3794,9 +3785,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>333720</xdr:colOff>
+      <xdr:colOff>333360</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>21240</xdr:rowOff>
+      <xdr:rowOff>20880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3805,7 +3796,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5637240" cy="2741400"/>
+        <a:ext cx="5636880" cy="2741040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3829,9 +3820,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>333720</xdr:colOff>
+      <xdr:colOff>333360</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>21240</xdr:rowOff>
+      <xdr:rowOff>20880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3840,7 +3831,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5637240" cy="2741400"/>
+        <a:ext cx="5636880" cy="2741040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3864,9 +3855,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>333720</xdr:colOff>
+      <xdr:colOff>333360</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>21240</xdr:rowOff>
+      <xdr:rowOff>20880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3875,7 +3866,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5637240" cy="2741400"/>
+        <a:ext cx="5636880" cy="2741040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3904,10 +3895,10 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.17004048583"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.0242914979757"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.5991902834008"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.3481781376518"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -4958,7 +4949,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="G33" activeCellId="0" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4966,8 +4957,8 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.2388663967611"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.8906882591093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.668016194332"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.9959514170041"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -5253,9 +5244,6 @@
       <c r="G24" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="H24" s="0" t="s">
-        <v>138</v>
-      </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
@@ -5264,23 +5252,23 @@
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>27</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>123</v>
@@ -5289,7 +5277,7 @@
         <v>124</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G29" s="0" t="s">
         <v>126</v>
@@ -5297,7 +5285,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>34</v>
@@ -5312,38 +5300,38 @@
         <v>124</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="C33" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="D33" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="E33" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="F33" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="E33" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="F33" s="0" t="s">
-        <v>153</v>
-      </c>
       <c r="G33" s="0" t="s">
-        <v>154</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update project product backlog
</commit_message>
<xml_diff>
--- a/Project/Clas Diagram and Backlog/Product Backlog.xlsx
+++ b/Project/Clas Diagram and Backlog/Product Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" state="visible" r:id="rId2"/>
@@ -487,11 +487,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="D\-MMM"/>
+    <numFmt numFmtId="166" formatCode="D\-MMM"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -531,6 +532,19 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="14"/>
       <color rgb="FF595959"/>
       <name val="Calibri"/>
@@ -549,7 +563,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -560,6 +574,84 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC00CC"/>
+        <bgColor rgb="FFFF0066"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66FF"/>
+        <bgColor rgb="FFFF6699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0000FF"/>
+        <bgColor rgb="FF0000FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6699FF"/>
+        <bgColor rgb="FF5B9BD5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008000"/>
+        <bgColor rgb="FF008080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FF66"/>
+        <bgColor rgb="FF99CC00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
+        <bgColor rgb="FFFF7C80"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9966"/>
+        <bgColor rgb="FFFF7C80"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0066"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7C80"/>
+        <bgColor rgb="FFFF6699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0066"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6699"/>
+        <bgColor rgb="FFFF7C80"/>
       </patternFill>
     </fill>
   </fills>
@@ -597,7 +689,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -610,6 +702,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -618,7 +714,63 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -643,7 +795,7 @@
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFCC00CC"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008000"/>
@@ -653,16 +805,16 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF5B9BD5"/>
+      <rgbColor rgb="FF6699FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FFFF7C80"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFD9D9D9"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFF0066"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800080"/>
@@ -674,17 +826,17 @@
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFF9966"/>
+      <rgbColor rgb="FFFF66FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF66FF66"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6699"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF595959"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF5B9BD5"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -698,7 +850,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -938,19 +1090,19 @@
                   <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -965,11 +1117,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="50193812"/>
-        <c:axId val="15727160"/>
+        <c:axId val="53858970"/>
+        <c:axId val="9803018"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="50193812"/>
+        <c:axId val="53858970"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1043,14 +1195,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15727160"/>
+        <c:crossAx val="9803018"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="15727160"/>
+        <c:axId val="9803018"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1131,7 +1283,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50193812"/>
+        <c:crossAx val="53858970"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1159,7 +1311,348 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>Product Backlog Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>label 0</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Left</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="5b9bd5"/>
+            </a:solidFill>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="5b9bd5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sprint 3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sprint 4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sprint 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>0</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="35039265"/>
+        <c:axId val="50864412"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="35039265"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Sprint Number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="MM/DD/YYYY" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="d9d9d9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="50864412"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50864412"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Features Left at End of Sprint</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="35039265"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1467,11 +1960,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="28544889"/>
-        <c:axId val="41106859"/>
+        <c:axId val="69297771"/>
+        <c:axId val="37769011"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="28544889"/>
+        <c:axId val="69297771"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1545,14 +2038,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41106859"/>
+        <c:crossAx val="37769011"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41106859"/>
+        <c:axId val="37769011"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1633,7 +2126,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28544889"/>
+        <c:crossAx val="69297771"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1661,7 +2154,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1969,11 +2462,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="71032889"/>
-        <c:axId val="16890469"/>
+        <c:axId val="91980035"/>
+        <c:axId val="84226556"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="71032889"/>
+        <c:axId val="91980035"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2047,14 +2540,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16890469"/>
+        <c:crossAx val="84226556"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="16890469"/>
+        <c:axId val="84226556"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2135,7 +2628,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71032889"/>
+        <c:crossAx val="91980035"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2163,7 +2656,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2471,11 +2964,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="49081331"/>
-        <c:axId val="4704043"/>
+        <c:axId val="69325847"/>
+        <c:axId val="66942493"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="49081331"/>
+        <c:axId val="69325847"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2549,14 +3042,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4704043"/>
+        <c:crossAx val="66942493"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="4704043"/>
+        <c:axId val="66942493"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2637,7 +3130,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49081331"/>
+        <c:crossAx val="69325847"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2665,7 +3158,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2973,11 +3466,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="8971600"/>
-        <c:axId val="8319402"/>
+        <c:axId val="87139306"/>
+        <c:axId val="24139619"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="8971600"/>
+        <c:axId val="87139306"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3051,14 +3544,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8319402"/>
+        <c:crossAx val="24139619"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="8319402"/>
+        <c:axId val="24139619"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3139,7 +3632,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8971600"/>
+        <c:crossAx val="87139306"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3167,7 +3660,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3475,11 +3968,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="67016042"/>
-        <c:axId val="25181228"/>
+        <c:axId val="23935037"/>
+        <c:axId val="38308392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="67016042"/>
+        <c:axId val="23935037"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3553,14 +4046,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25181228"/>
+        <c:crossAx val="38308392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="25181228"/>
+        <c:axId val="38308392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3641,7 +4134,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67016042"/>
+        <c:crossAx val="23935037"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3674,15 +4167,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>647640</xdr:colOff>
+      <xdr:colOff>704880</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>87480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>203400</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>85320</xdr:rowOff>
+      <xdr:colOff>631440</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>24120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3690,12 +4183,42 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5762520" y="87480"/>
-        <a:ext cx="12109680" cy="2741040"/>
+        <a:off x="5771880" y="87480"/>
+        <a:ext cx="12175920" cy="2740680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>647640</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>80640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>205200</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>80280</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="5714640" y="80640"/>
+        <a:ext cx="11806920" cy="2628360"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3715,18 +4238,18 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>5760</xdr:colOff>
+      <xdr:colOff>5400</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>43920</xdr:rowOff>
+      <xdr:rowOff>43560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2916360" y="23040"/>
-        <a:ext cx="7719120" cy="2748600"/>
+        <a:ext cx="7766280" cy="2748240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3750,18 +4273,18 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>333360</xdr:colOff>
+      <xdr:colOff>333000</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>20880</xdr:rowOff>
+      <xdr:rowOff>20520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5636880" cy="2741040"/>
+        <a:ext cx="5636520" cy="2740680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3785,18 +4308,18 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>333360</xdr:colOff>
+      <xdr:colOff>333000</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>20880</xdr:rowOff>
+      <xdr:rowOff>20520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 1"/>
+        <xdr:cNvPr id="4" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5636880" cy="2741040"/>
+        <a:ext cx="5636520" cy="2740680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3820,18 +4343,18 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>333360</xdr:colOff>
+      <xdr:colOff>333000</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>20880</xdr:rowOff>
+      <xdr:rowOff>20520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 1"/>
+        <xdr:cNvPr id="5" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5636880" cy="2741040"/>
+        <a:ext cx="5636520" cy="2740680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3855,18 +4378,18 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>333360</xdr:colOff>
+      <xdr:colOff>333000</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>20880</xdr:rowOff>
+      <xdr:rowOff>20520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 1"/>
+        <xdr:cNvPr id="6" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5636880" cy="2741040"/>
+        <a:ext cx="5636520" cy="2740680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3886,47 +4409,49 @@
   </sheetPr>
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.5991902834008"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.3481781376518"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.8825910931174"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.5263157894737"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>4</v>
       </c>
@@ -3943,7 +4468,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>9</v>
       </c>
@@ -3959,52 +4484,51 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="0" t="n">
         <f aca="false">C8-D9</f>
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C9" s="0" t="n">
         <f aca="false">COUNT(B21:B104)</f>
         <v>28</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E9" s="2" t="n">
         <v>43189</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="0" t="n">
         <f aca="false">C9-D10</f>
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C10" s="0" t="n">
         <f aca="false">COUNT(B21:B105)</f>
         <v>28</v>
       </c>
       <c r="D10" s="1" t="n">
-        <f aca="false">D9</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E10" s="2" t="n">
         <v>43198</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">C10-D11</f>
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C11" s="0" t="n">
         <f aca="false">COUNT(B21:B106)</f>
@@ -4012,19 +4536,19 @@
       </c>
       <c r="D11" s="1" t="n">
         <f aca="false">D10</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E11" s="2" t="n">
         <v>43205</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="0" t="n">
         <f aca="false">C11-D12</f>
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C12" s="0" t="n">
         <f aca="false">COUNT(B21:B107)</f>
@@ -4032,19 +4556,19 @@
       </c>
       <c r="D12" s="1" t="n">
         <f aca="false">D11</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E12" s="2" t="n">
         <v>43212</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="0" t="n">
         <f aca="false">C12-D13</f>
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C13" s="0" t="n">
         <f aca="false">COUNT(B21:B108)</f>
@@ -4052,29 +4576,30 @@
       </c>
       <c r="D13" s="1" t="n">
         <f aca="false">D12</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E13" s="2" t="n">
         <v>43219</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D14" s="3"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4"/>
-    </row>
-    <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>17</v>
       </c>
@@ -4106,826 +4631,782 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+    <row r="21" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="0" t="n">
+      <c r="B21" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="E21" s="1" t="n">
+      <c r="E21" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="F21" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G21" s="0" t="s">
+      <c r="G21" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H21" s="0" t="s">
+      <c r="H21" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I21" s="0" t="s">
+      <c r="I21" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="J21" s="0" t="s">
+      <c r="J21" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
+    <row r="22" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="0" t="n">
+      <c r="B22" s="7" t="n">
         <f aca="false">B21+1</f>
         <v>2</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="D22" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="E22" s="1" t="n">
+      <c r="E22" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="F22" s="0" t="s">
+      <c r="F22" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G22" s="0" t="s">
+      <c r="G22" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H22" s="0" t="s">
+      <c r="H22" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="I22" s="0" t="s">
+      <c r="I22" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="J22" s="0" t="s">
+      <c r="J22" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1"/>
-      <c r="B23" s="0" t="n">
+    <row r="23" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="6" t="n">
         <f aca="false">B22+1</f>
         <v>3</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="D23" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="E23" s="1" t="n">
+      <c r="E23" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="F23" s="0" t="s">
+      <c r="F23" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G23" s="0" t="s">
+      <c r="G23" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="H23" s="0" t="s">
+      <c r="H23" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="I23" s="0" t="s">
+      <c r="I23" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="J23" s="0" t="s">
+      <c r="J23" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1"/>
-      <c r="B24" s="0" t="n">
+    <row r="24" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="7" t="n">
         <f aca="false">B23+1</f>
         <v>4</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="0" t="n">
+      <c r="D24" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="E24" s="1" t="n">
+      <c r="E24" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="F24" s="0" t="s">
+      <c r="F24" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G24" s="0" t="s">
+      <c r="G24" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H24" s="0" t="s">
+      <c r="H24" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="I24" s="0" t="s">
+      <c r="I24" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="J24" s="0" t="s">
+      <c r="J24" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1"/>
-      <c r="B25" s="0" t="n">
+    <row r="25" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="8" t="n">
         <f aca="false">B24+1</f>
         <v>5</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="D25" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="0" t="s">
+      <c r="E25" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F25" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G25" s="0" t="s">
+      <c r="G25" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="H25" s="0" t="s">
+      <c r="H25" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="I25" s="0" t="s">
+      <c r="I25" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="J25" s="0" t="s">
+      <c r="J25" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1"/>
-      <c r="B26" s="0" t="n">
+    <row r="26" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="9" t="n">
         <f aca="false">B25+1</f>
         <v>6</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D26" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="E26" s="1"/>
-      <c r="F26" s="0" t="s">
+      <c r="E26" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F26" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G26" s="0" t="s">
+      <c r="G26" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="H26" s="0" t="s">
+      <c r="H26" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="I26" s="0" t="s">
+      <c r="I26" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="J26" s="0" t="s">
+      <c r="J26" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1"/>
-      <c r="B27" s="0" t="n">
+    <row r="27" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="8" t="n">
         <f aca="false">B26+1</f>
         <v>7</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="D27" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="E27" s="1"/>
-      <c r="F27" s="0" t="s">
+      <c r="F27" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G27" s="0" t="s">
+      <c r="G27" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="H27" s="0" t="s">
+      <c r="H27" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="I27" s="0" t="s">
+      <c r="I27" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="J27" s="0" t="s">
+      <c r="J27" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1"/>
-      <c r="B28" s="0" t="n">
+    <row r="28" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="9" t="n">
         <f aca="false">B27+1</f>
         <v>8</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="0" t="n">
+      <c r="D28" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="E28" s="1"/>
-      <c r="F28" s="0" t="s">
+      <c r="F28" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="G28" s="0" t="s">
+      <c r="G28" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="H28" s="0" t="s">
+      <c r="H28" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="I28" s="0" t="s">
+      <c r="I28" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="J28" s="0" t="s">
+      <c r="J28" s="9" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1"/>
-      <c r="B29" s="0" t="n">
+    <row r="29" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="8" t="n">
         <f aca="false">B28+1</f>
         <v>9</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="0" t="n">
+      <c r="D29" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="E29" s="1"/>
-      <c r="F29" s="0" t="s">
+      <c r="F29" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G29" s="0" t="s">
+      <c r="G29" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="H29" s="0" t="s">
+      <c r="H29" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="I29" s="0" t="s">
+      <c r="I29" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="J29" s="0" t="s">
+      <c r="J29" s="8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1"/>
-      <c r="B30" s="0" t="n">
+    <row r="30" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="9" t="n">
         <f aca="false">B29+1</f>
         <v>10</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="0" t="n">
+      <c r="D30" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="E30" s="1"/>
-      <c r="F30" s="0" t="s">
+      <c r="F30" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G30" s="0" t="s">
+      <c r="G30" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="H30" s="0" t="s">
+      <c r="H30" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="I30" s="0" t="s">
+      <c r="I30" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="J30" s="0" t="s">
+      <c r="J30" s="9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1"/>
-      <c r="B31" s="0" t="n">
+    <row r="31" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="10" t="n">
         <f aca="false">B30+1</f>
         <v>11</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="0" t="n">
+      <c r="D31" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="E31" s="1"/>
-      <c r="F31" s="0" t="s">
+      <c r="F31" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="G31" s="0" t="s">
+      <c r="G31" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="H31" s="0" t="s">
+      <c r="H31" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="I31" s="0" t="s">
+      <c r="I31" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="J31" s="0" t="s">
+      <c r="J31" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1"/>
-      <c r="B32" s="0" t="n">
+    <row r="32" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="11" t="n">
         <f aca="false">B31+1</f>
         <v>12</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D32" s="0" t="n">
+      <c r="D32" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="E32" s="1"/>
-      <c r="F32" s="0" t="s">
+      <c r="F32" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G32" s="0" t="s">
+      <c r="G32" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="H32" s="0" t="s">
+      <c r="H32" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="I32" s="0" t="s">
+      <c r="I32" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="J32" s="0" t="s">
+      <c r="J32" s="11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1"/>
-      <c r="B33" s="0" t="n">
+    <row r="33" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="10" t="n">
         <f aca="false">B32+1</f>
         <v>13</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D33" s="0" t="n">
+      <c r="D33" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="E33" s="1"/>
-      <c r="F33" s="0" t="s">
+      <c r="F33" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G33" s="0" t="s">
+      <c r="G33" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="H33" s="0" t="s">
+      <c r="H33" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="I33" s="0" t="s">
+      <c r="I33" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="J33" s="0" t="s">
+      <c r="J33" s="10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1"/>
-      <c r="B34" s="0" t="n">
+    <row r="34" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="12" t="n">
         <f aca="false">B33+1</f>
         <v>14</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D34" s="0" t="n">
+      <c r="D34" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="E34" s="1"/>
-      <c r="F34" s="0" t="s">
+      <c r="F34" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="G34" s="0" t="s">
+      <c r="G34" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="H34" s="0" t="s">
+      <c r="H34" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="I34" s="0" t="s">
+      <c r="I34" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="J34" s="0" t="s">
+      <c r="J34" s="12" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1"/>
-      <c r="B35" s="0" t="n">
+    <row r="35" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="13" t="n">
         <f aca="false">B34+1</f>
         <v>15</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D35" s="0" t="n">
+      <c r="D35" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="E35" s="1"/>
-      <c r="F35" s="0" t="s">
+      <c r="F35" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="G35" s="0" t="s">
+      <c r="G35" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="H35" s="0" t="s">
+      <c r="H35" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="I35" s="0" t="s">
+      <c r="I35" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="J35" s="0" t="s">
+      <c r="J35" s="13" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1"/>
-      <c r="B36" s="0" t="n">
+    <row r="36" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="12" t="n">
         <f aca="false">B35+1</f>
         <v>16</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D36" s="0" t="n">
+      <c r="D36" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="E36" s="1"/>
-      <c r="F36" s="0" t="s">
+      <c r="F36" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="G36" s="0" t="s">
+      <c r="G36" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="H36" s="0" t="s">
+      <c r="H36" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="I36" s="0" t="s">
+      <c r="I36" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="J36" s="0" t="s">
+      <c r="J36" s="12" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1"/>
-      <c r="B37" s="0" t="n">
+    <row r="37" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="13" t="n">
         <f aca="false">B36+1</f>
         <v>17</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D37" s="0" t="n">
+      <c r="D37" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="E37" s="1"/>
-      <c r="F37" s="0" t="s">
+      <c r="F37" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="G37" s="0" t="s">
+      <c r="G37" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="H37" s="0" t="s">
+      <c r="H37" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="I37" s="0" t="s">
+      <c r="I37" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="J37" s="0" t="s">
+      <c r="J37" s="13" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1"/>
-      <c r="B38" s="0" t="n">
+    <row r="38" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="12" t="n">
         <f aca="false">B37+1</f>
         <v>18</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D38" s="0" t="n">
+      <c r="D38" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="E38" s="1"/>
-      <c r="F38" s="0" t="s">
+      <c r="F38" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="G38" s="0" t="s">
+      <c r="G38" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="H38" s="0" t="s">
+      <c r="H38" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="I38" s="0" t="s">
+      <c r="I38" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="J38" s="0" t="s">
+      <c r="J38" s="12" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1"/>
-      <c r="B39" s="0" t="n">
+    <row r="39" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="13" t="n">
         <f aca="false">B38+1</f>
         <v>19</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D39" s="0" t="n">
+      <c r="D39" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="E39" s="1"/>
-      <c r="F39" s="0" t="s">
+      <c r="F39" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="G39" s="0" t="s">
+      <c r="G39" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="H39" s="0" t="s">
+      <c r="H39" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="I39" s="0" t="s">
+      <c r="I39" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="J39" s="0" t="s">
+      <c r="J39" s="13" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1"/>
-      <c r="B40" s="0" t="n">
+    <row r="40" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="14" t="n">
         <f aca="false">B39+1</f>
         <v>20</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D40" s="0" t="n">
+      <c r="D40" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="E40" s="1"/>
-      <c r="F40" s="0" t="s">
+      <c r="F40" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G40" s="0" t="s">
+      <c r="G40" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="H40" s="0" t="s">
+      <c r="H40" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="I40" s="0" t="s">
+      <c r="I40" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="J40" s="0" t="s">
+      <c r="J40" s="14" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1"/>
-      <c r="B41" s="0" t="n">
+    <row r="41" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="15" t="n">
         <f aca="false">B40+1</f>
         <v>21</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D41" s="0" t="n">
+      <c r="D41" s="15" t="n">
         <v>5</v>
       </c>
-      <c r="E41" s="1"/>
-      <c r="F41" s="0" t="s">
+      <c r="F41" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="G41" s="0" t="s">
+      <c r="G41" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="H41" s="0" t="s">
+      <c r="H41" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="I41" s="0" t="s">
+      <c r="I41" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="J41" s="0" t="s">
+      <c r="J41" s="15" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1"/>
-      <c r="B42" s="0" t="n">
+    <row r="42" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="14" t="n">
         <f aca="false">B41+1</f>
         <v>22</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D42" s="0" t="n">
+      <c r="D42" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="E42" s="1"/>
-      <c r="F42" s="0" t="s">
+      <c r="F42" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G42" s="0" t="s">
+      <c r="G42" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="H42" s="0" t="s">
+      <c r="H42" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="I42" s="0" t="s">
+      <c r="I42" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="J42" s="0" t="s">
+      <c r="J42" s="14" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1"/>
-      <c r="B43" s="0" t="n">
+    <row r="43" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="16" t="n">
         <f aca="false">B42+1</f>
         <v>23</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D43" s="0" t="n">
+      <c r="D43" s="16" t="n">
         <v>6</v>
       </c>
-      <c r="E43" s="1"/>
-      <c r="F43" s="0" t="s">
+      <c r="F43" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="G43" s="0" t="s">
+      <c r="G43" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="H43" s="0" t="s">
+      <c r="H43" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="I43" s="0" t="s">
+      <c r="I43" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="J43" s="0" t="s">
+      <c r="J43" s="16" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1"/>
-      <c r="B44" s="0" t="n">
+    <row r="44" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="17" t="n">
         <f aca="false">B43+1</f>
         <v>24</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D44" s="0" t="n">
+      <c r="D44" s="17" t="n">
         <v>6</v>
       </c>
-      <c r="E44" s="1"/>
-      <c r="F44" s="0" t="s">
+      <c r="F44" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="G44" s="0" t="s">
+      <c r="G44" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="H44" s="0" t="s">
+      <c r="H44" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="I44" s="0" t="s">
+      <c r="I44" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="J44" s="0" t="s">
+      <c r="J44" s="17" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1"/>
-      <c r="B45" s="0" t="n">
+    <row r="45" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="16" t="n">
         <f aca="false">B44+1</f>
         <v>25</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D45" s="0" t="n">
+      <c r="D45" s="16" t="n">
         <v>6</v>
       </c>
-      <c r="E45" s="1"/>
-      <c r="F45" s="0" t="s">
+      <c r="F45" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="G45" s="0" t="s">
+      <c r="G45" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="H45" s="0" t="s">
+      <c r="H45" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="I45" s="0" t="s">
+      <c r="I45" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="J45" s="0" t="s">
+      <c r="J45" s="16" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1"/>
-      <c r="B46" s="0" t="n">
+    <row r="46" s="18" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="18" t="n">
         <f aca="false">B45+1</f>
         <v>26</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D46" s="0" t="n">
+      <c r="D46" s="18" t="n">
         <v>7</v>
       </c>
-      <c r="E46" s="1"/>
-      <c r="F46" s="0" t="s">
+      <c r="F46" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="G46" s="0" t="s">
+      <c r="G46" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="H46" s="0" t="s">
+      <c r="H46" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="I46" s="0" t="s">
+      <c r="I46" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="J46" s="0" t="s">
+      <c r="J46" s="18" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1"/>
-      <c r="B47" s="0" t="n">
+    <row r="47" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="19" t="n">
         <f aca="false">B46+1</f>
         <v>27</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D47" s="0" t="n">
+      <c r="D47" s="19" t="n">
         <v>7</v>
       </c>
-      <c r="E47" s="1"/>
-      <c r="F47" s="0" t="s">
+      <c r="F47" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="G47" s="0" t="s">
+      <c r="G47" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="H47" s="0" t="s">
+      <c r="H47" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="I47" s="0" t="s">
+      <c r="I47" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="J47" s="0" t="s">
+      <c r="J47" s="19" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1"/>
-      <c r="B48" s="0" t="n">
+    <row r="48" s="18" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="18" t="n">
         <f aca="false">B47+1</f>
         <v>28</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D48" s="0" t="n">
+      <c r="D48" s="18" t="n">
         <v>7</v>
       </c>
-      <c r="E48" s="1"/>
-      <c r="F48" s="0" t="s">
+      <c r="F48" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="G48" s="0" t="s">
+      <c r="G48" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="H48" s="0" t="s">
+      <c r="H48" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="I48" s="0" t="s">
+      <c r="I48" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="J48" s="0" t="s">
+      <c r="J48" s="18" t="s">
         <v>106</v>
       </c>
     </row>
@@ -4948,7 +5429,7 @@
   </sheetPr>
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G33" activeCellId="0" sqref="G33"/>
     </sheetView>
   </sheetViews>
@@ -4957,8 +5438,8 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.668016194332"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="51.0971659919028"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.1052631578947"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -4974,7 +5455,7 @@
       <c r="A2" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="5" t="n">
+      <c r="B2" s="20" t="n">
         <v>43183</v>
       </c>
     </row>
@@ -4982,7 +5463,7 @@
       <c r="A3" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="5" t="n">
+      <c r="B3" s="20" t="n">
         <v>43189</v>
       </c>
     </row>
@@ -5100,7 +5581,7 @@
       <c r="F18" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="21" t="s">
         <v>126</v>
       </c>
       <c r="H18" s="0" t="s">
@@ -5375,7 +5856,7 @@
       <c r="A2" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="5" t="n">
+      <c r="B2" s="20" t="n">
         <v>43192</v>
       </c>
     </row>
@@ -5383,7 +5864,7 @@
       <c r="A3" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="5" t="n">
+      <c r="B3" s="20" t="n">
         <v>43198</v>
       </c>
     </row>
@@ -5526,7 +6007,7 @@
       <c r="A2" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="5" t="n">
+      <c r="B2" s="20" t="n">
         <v>43199</v>
       </c>
     </row>
@@ -5534,7 +6015,7 @@
       <c r="A3" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="5" t="n">
+      <c r="B3" s="20" t="n">
         <v>43205</v>
       </c>
     </row>
@@ -5677,7 +6158,7 @@
       <c r="A2" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="5" t="n">
+      <c r="B2" s="20" t="n">
         <v>43206</v>
       </c>
     </row>
@@ -5685,7 +6166,7 @@
       <c r="A3" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="5" t="n">
+      <c r="B3" s="20" t="n">
         <v>43212</v>
       </c>
     </row>
@@ -5828,7 +6309,7 @@
       <c r="A2" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="5" t="n">
+      <c r="B2" s="20" t="n">
         <v>43213</v>
       </c>
     </row>
@@ -5836,7 +6317,7 @@
       <c r="A3" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="5" t="n">
+      <c r="B3" s="20" t="n">
         <v>43219</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated product backlog file
</commit_message>
<xml_diff>
--- a/Project/Clas Diagram and Backlog/Product Backlog.xlsx
+++ b/Project/Clas Diagram and Backlog/Product Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" state="visible" r:id="rId2"/>
@@ -487,10 +487,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="D\-MMM"/>
-    <numFmt numFmtId="166" formatCode="D\-MMM"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -689,7 +688,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -699,10 +698,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -770,7 +765,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -850,7 +845,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1117,11 +1112,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="53858970"/>
-        <c:axId val="9803018"/>
+        <c:axId val="29913391"/>
+        <c:axId val="28593772"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="53858970"/>
+        <c:axId val="29913391"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1195,14 +1190,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9803018"/>
+        <c:crossAx val="28593772"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="9803018"/>
+        <c:axId val="28593772"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1283,7 +1278,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53858970"/>
+        <c:crossAx val="29913391"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1311,7 +1306,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1386,6 +1381,78 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
@@ -1458,11 +1525,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="35039265"/>
-        <c:axId val="50864412"/>
+        <c:axId val="8971771"/>
+        <c:axId val="33950855"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="35039265"/>
+        <c:axId val="8971771"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1536,14 +1603,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50864412"/>
+        <c:crossAx val="33950855"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50864412"/>
+        <c:axId val="33950855"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1624,7 +1691,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35039265"/>
+        <c:crossAx val="8971771"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1652,7 +1719,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1960,11 +2027,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="69297771"/>
-        <c:axId val="37769011"/>
+        <c:axId val="21487886"/>
+        <c:axId val="72306409"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="69297771"/>
+        <c:axId val="21487886"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2038,14 +2105,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37769011"/>
+        <c:crossAx val="72306409"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="37769011"/>
+        <c:axId val="72306409"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2126,7 +2193,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69297771"/>
+        <c:crossAx val="21487886"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2154,7 +2221,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2462,11 +2529,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="91980035"/>
-        <c:axId val="84226556"/>
+        <c:axId val="38507833"/>
+        <c:axId val="45453091"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="91980035"/>
+        <c:axId val="38507833"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2540,14 +2607,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84226556"/>
+        <c:crossAx val="45453091"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84226556"/>
+        <c:axId val="45453091"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2628,7 +2695,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91980035"/>
+        <c:crossAx val="38507833"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2656,7 +2723,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2964,11 +3031,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="69325847"/>
-        <c:axId val="66942493"/>
+        <c:axId val="22475482"/>
+        <c:axId val="24613651"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="69325847"/>
+        <c:axId val="22475482"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3042,14 +3109,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66942493"/>
+        <c:crossAx val="24613651"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66942493"/>
+        <c:axId val="24613651"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3130,7 +3197,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69325847"/>
+        <c:crossAx val="22475482"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3158,7 +3225,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3466,11 +3533,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="87139306"/>
-        <c:axId val="24139619"/>
+        <c:axId val="44872336"/>
+        <c:axId val="18970411"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="87139306"/>
+        <c:axId val="44872336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3544,14 +3611,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="24139619"/>
+        <c:crossAx val="18970411"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="24139619"/>
+        <c:axId val="18970411"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3632,7 +3699,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87139306"/>
+        <c:crossAx val="44872336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3660,7 +3727,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3968,11 +4035,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="23935037"/>
-        <c:axId val="38308392"/>
+        <c:axId val="91664581"/>
+        <c:axId val="11799980"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="23935037"/>
+        <c:axId val="91664581"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4046,14 +4113,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38308392"/>
+        <c:crossAx val="11799980"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="38308392"/>
+        <c:axId val="11799980"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4134,7 +4201,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23935037"/>
+        <c:crossAx val="91664581"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4173,9 +4240,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>631440</xdr:colOff>
+      <xdr:colOff>631080</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>24120</xdr:rowOff>
+      <xdr:rowOff>23760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4183,8 +4250,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5771880" y="87480"/>
-        <a:ext cx="12175920" cy="2740680"/>
+        <a:off x="5781600" y="87480"/>
+        <a:ext cx="12251520" cy="2740320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4203,9 +4270,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>205200</xdr:colOff>
+      <xdr:colOff>204840</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>80280</xdr:rowOff>
+      <xdr:rowOff>79920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4213,8 +4280,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5714640" y="80640"/>
-        <a:ext cx="11806920" cy="2628360"/>
+        <a:off x="5724360" y="80640"/>
+        <a:ext cx="11882520" cy="2628000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4238,9 +4305,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>5400</xdr:colOff>
+      <xdr:colOff>5040</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>43560</xdr:rowOff>
+      <xdr:rowOff>43200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4249,7 +4316,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2916360" y="23040"/>
-        <a:ext cx="7766280" cy="2748240"/>
+        <a:ext cx="7813800" cy="2747880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4273,9 +4340,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>333000</xdr:colOff>
+      <xdr:colOff>332640</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>20520</xdr:rowOff>
+      <xdr:rowOff>20160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4284,7 +4351,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5636520" cy="2740680"/>
+        <a:ext cx="5636160" cy="2740320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4308,9 +4375,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>333000</xdr:colOff>
+      <xdr:colOff>332640</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>20520</xdr:rowOff>
+      <xdr:rowOff>20160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4319,7 +4386,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5636520" cy="2740680"/>
+        <a:ext cx="5636160" cy="2740320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4343,9 +4410,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>333000</xdr:colOff>
+      <xdr:colOff>332640</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>20520</xdr:rowOff>
+      <xdr:rowOff>20160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4354,7 +4421,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5636520" cy="2740680"/>
+        <a:ext cx="5636160" cy="2740320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4378,9 +4445,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>333000</xdr:colOff>
+      <xdr:colOff>332640</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>20520</xdr:rowOff>
+      <xdr:rowOff>20160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4389,7 +4456,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5636520" cy="2740680"/>
+        <a:ext cx="5636160" cy="2740320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4418,10 +4485,10 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.96356275303644"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.8825910931174"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.5263157894737"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.2064777327935"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.9554655870445"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.57085020242915"/>
@@ -4583,21 +4650,20 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="3"/>
       <c r="E14" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5"/>
+      <c r="A19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
@@ -4631,782 +4697,782 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="6" t="s">
+    <row r="21" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="6" t="n">
+      <c r="B21" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="6" t="n">
+      <c r="D21" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E21" s="6" t="n">
+      <c r="E21" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="H21" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="I21" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J21" s="6" t="s">
+      <c r="J21" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7" t="s">
+    <row r="22" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="7" t="n">
+      <c r="B22" s="6" t="n">
         <f aca="false">B21+1</f>
         <v>2</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="7" t="n">
+      <c r="D22" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="E22" s="7" t="n">
+      <c r="E22" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G22" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H22" s="7" t="s">
+      <c r="H22" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="I22" s="7" t="s">
+      <c r="I22" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="J22" s="7" t="s">
+      <c r="J22" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="6" t="n">
+    <row r="23" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="5" t="n">
         <f aca="false">B22+1</f>
         <v>3</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="6" t="n">
+      <c r="D23" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E23" s="6" t="n">
+      <c r="E23" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="G23" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H23" s="6" t="s">
+      <c r="H23" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I23" s="6" t="s">
+      <c r="I23" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J23" s="6" t="s">
+      <c r="J23" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="7" t="n">
+    <row r="24" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="6" t="n">
         <f aca="false">B23+1</f>
         <v>4</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="7" t="n">
+      <c r="D24" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="E24" s="7" t="n">
+      <c r="E24" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G24" s="7" t="s">
+      <c r="G24" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="H24" s="7" t="s">
+      <c r="H24" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="I24" s="7" t="s">
+      <c r="I24" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="J24" s="7" t="s">
+      <c r="J24" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="8" t="n">
+    <row r="25" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="7" t="n">
         <f aca="false">B24+1</f>
         <v>5</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="8" t="n">
+      <c r="D25" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="E25" s="8" t="n">
+      <c r="E25" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="F25" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G25" s="8" t="s">
+      <c r="G25" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="H25" s="8" t="s">
+      <c r="H25" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="I25" s="8" t="s">
+      <c r="I25" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="J25" s="8" t="s">
+      <c r="J25" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="9" t="n">
+    <row r="26" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="8" t="n">
         <f aca="false">B25+1</f>
         <v>6</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="9" t="n">
+      <c r="D26" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="E26" s="9" t="n">
+      <c r="E26" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="F26" s="9" t="s">
+      <c r="F26" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G26" s="9" t="s">
+      <c r="G26" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="H26" s="9" t="s">
+      <c r="H26" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="I26" s="9" t="s">
+      <c r="I26" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="J26" s="9" t="s">
+      <c r="J26" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="27" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="8" t="n">
+    <row r="27" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="7" t="n">
         <f aca="false">B26+1</f>
         <v>7</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="8" t="n">
+      <c r="D27" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F27" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G27" s="8" t="s">
+      <c r="G27" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="H27" s="8" t="s">
+      <c r="H27" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="I27" s="8" t="s">
+      <c r="I27" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="J27" s="8" t="s">
+      <c r="J27" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="28" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="9" t="n">
+    <row r="28" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="8" t="n">
         <f aca="false">B27+1</f>
         <v>8</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="9" t="n">
+      <c r="D28" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="F28" s="9" t="s">
+      <c r="F28" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G28" s="9" t="s">
+      <c r="G28" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="H28" s="9" t="s">
+      <c r="H28" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="I28" s="9" t="s">
+      <c r="I28" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="J28" s="9" t="s">
+      <c r="J28" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="8" t="n">
+    <row r="29" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="7" t="n">
         <f aca="false">B28+1</f>
         <v>9</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="8" t="n">
+      <c r="D29" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="F29" s="8" t="s">
+      <c r="F29" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G29" s="8" t="s">
+      <c r="G29" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="H29" s="8" t="s">
+      <c r="H29" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="I29" s="8" t="s">
+      <c r="I29" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="J29" s="8" t="s">
+      <c r="J29" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="30" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="9" t="n">
+    <row r="30" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="8" t="n">
         <f aca="false">B29+1</f>
         <v>10</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="9" t="n">
+      <c r="D30" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="F30" s="9" t="s">
+      <c r="F30" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G30" s="9" t="s">
+      <c r="G30" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="H30" s="9" t="s">
+      <c r="H30" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="I30" s="9" t="s">
+      <c r="I30" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="J30" s="9" t="s">
+      <c r="J30" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="31" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="10" t="n">
+    <row r="31" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="9" t="n">
         <f aca="false">B30+1</f>
         <v>11</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="10" t="n">
+      <c r="D31" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="F31" s="10" t="s">
+      <c r="F31" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="G31" s="10" t="s">
+      <c r="G31" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H31" s="10" t="s">
+      <c r="H31" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="I31" s="10" t="s">
+      <c r="I31" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="J31" s="10" t="s">
+      <c r="J31" s="9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="32" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="11" t="n">
+    <row r="32" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="10" t="n">
         <f aca="false">B31+1</f>
         <v>12</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D32" s="11" t="n">
+      <c r="D32" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="F32" s="11" t="s">
+      <c r="F32" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G32" s="11" t="s">
+      <c r="G32" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="H32" s="11" t="s">
+      <c r="H32" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="I32" s="11" t="s">
+      <c r="I32" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="J32" s="11" t="s">
+      <c r="J32" s="10" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="33" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="10" t="n">
+    <row r="33" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="9" t="n">
         <f aca="false">B32+1</f>
         <v>13</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D33" s="10" t="n">
+      <c r="D33" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="F33" s="10" t="s">
+      <c r="F33" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G33" s="10" t="s">
+      <c r="G33" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="H33" s="10" t="s">
+      <c r="H33" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="I33" s="10" t="s">
+      <c r="I33" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="J33" s="10" t="s">
+      <c r="J33" s="9" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="34" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="12" t="n">
+    <row r="34" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="11" t="n">
         <f aca="false">B33+1</f>
         <v>14</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D34" s="12" t="n">
+      <c r="D34" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="F34" s="12" t="s">
+      <c r="F34" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G34" s="12" t="s">
+      <c r="G34" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="H34" s="12" t="s">
+      <c r="H34" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I34" s="12" t="s">
+      <c r="I34" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="J34" s="12" t="s">
+      <c r="J34" s="11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="35" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="13" t="n">
+    <row r="35" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="12" t="n">
         <f aca="false">B34+1</f>
         <v>15</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D35" s="13" t="n">
+      <c r="D35" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="F35" s="13" t="s">
+      <c r="F35" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="G35" s="13" t="s">
+      <c r="G35" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="H35" s="13" t="s">
+      <c r="H35" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="I35" s="13" t="s">
+      <c r="I35" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="J35" s="13" t="s">
+      <c r="J35" s="12" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="36" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="12" t="n">
+    <row r="36" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="11" t="n">
         <f aca="false">B35+1</f>
         <v>16</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C36" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D36" s="12" t="n">
+      <c r="D36" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="F36" s="12" t="s">
+      <c r="F36" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="G36" s="12" t="s">
+      <c r="G36" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="H36" s="12" t="s">
+      <c r="H36" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="I36" s="12" t="s">
+      <c r="I36" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="J36" s="12" t="s">
+      <c r="J36" s="11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="37" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="13" t="n">
+    <row r="37" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="12" t="n">
         <f aca="false">B36+1</f>
         <v>17</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C37" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D37" s="13" t="n">
+      <c r="D37" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="F37" s="13" t="s">
+      <c r="F37" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="G37" s="13" t="s">
+      <c r="G37" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="H37" s="13" t="s">
+      <c r="H37" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="I37" s="13" t="s">
+      <c r="I37" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="J37" s="13" t="s">
+      <c r="J37" s="12" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="38" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="12" t="n">
+    <row r="38" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="11" t="n">
         <f aca="false">B37+1</f>
         <v>18</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C38" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D38" s="12" t="n">
+      <c r="D38" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="F38" s="12" t="s">
+      <c r="F38" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="G38" s="12" t="s">
+      <c r="G38" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="H38" s="12" t="s">
+      <c r="H38" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="I38" s="12" t="s">
+      <c r="I38" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="J38" s="12" t="s">
+      <c r="J38" s="11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="39" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="13" t="n">
+    <row r="39" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="12" t="n">
         <f aca="false">B38+1</f>
         <v>19</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D39" s="13" t="n">
+      <c r="D39" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="F39" s="13" t="s">
+      <c r="F39" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="G39" s="13" t="s">
+      <c r="G39" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="H39" s="13" t="s">
+      <c r="H39" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="I39" s="13" t="s">
+      <c r="I39" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="J39" s="13" t="s">
+      <c r="J39" s="12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="40" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="14" t="n">
+    <row r="40" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="13" t="n">
         <f aca="false">B39+1</f>
         <v>20</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C40" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D40" s="14" t="n">
+      <c r="D40" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="F40" s="14" t="s">
+      <c r="F40" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="G40" s="14" t="s">
+      <c r="G40" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="H40" s="14" t="s">
+      <c r="H40" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="I40" s="14" t="s">
+      <c r="I40" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="J40" s="14" t="s">
+      <c r="J40" s="13" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="41" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="15" t="n">
+    <row r="41" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="14" t="n">
         <f aca="false">B40+1</f>
         <v>21</v>
       </c>
-      <c r="C41" s="15" t="s">
+      <c r="C41" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D41" s="15" t="n">
+      <c r="D41" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="F41" s="15" t="s">
+      <c r="F41" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G41" s="15" t="s">
+      <c r="G41" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="H41" s="15" t="s">
+      <c r="H41" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="I41" s="15" t="s">
+      <c r="I41" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="J41" s="15" t="s">
+      <c r="J41" s="14" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="42" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="14" t="n">
+    <row r="42" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="13" t="n">
         <f aca="false">B41+1</f>
         <v>22</v>
       </c>
-      <c r="C42" s="14" t="s">
+      <c r="C42" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D42" s="14" t="n">
+      <c r="D42" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="F42" s="14" t="s">
+      <c r="F42" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="G42" s="14" t="s">
+      <c r="G42" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="H42" s="14" t="s">
+      <c r="H42" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="I42" s="14" t="s">
+      <c r="I42" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="J42" s="14" t="s">
+      <c r="J42" s="13" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="43" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="16" t="n">
+    <row r="43" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="15" t="n">
         <f aca="false">B42+1</f>
         <v>23</v>
       </c>
-      <c r="C43" s="16" t="s">
+      <c r="C43" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D43" s="16" t="n">
+      <c r="D43" s="15" t="n">
         <v>6</v>
       </c>
-      <c r="F43" s="16" t="s">
+      <c r="F43" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="G43" s="16" t="s">
+      <c r="G43" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="H43" s="16" t="s">
+      <c r="H43" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="I43" s="16" t="s">
+      <c r="I43" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="J43" s="16" t="s">
+      <c r="J43" s="15" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="44" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="17" t="n">
+    <row r="44" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="16" t="n">
         <f aca="false">B43+1</f>
         <v>24</v>
       </c>
-      <c r="C44" s="17" t="s">
+      <c r="C44" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D44" s="17" t="n">
+      <c r="D44" s="16" t="n">
         <v>6</v>
       </c>
-      <c r="F44" s="17" t="s">
+      <c r="F44" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="G44" s="17" t="s">
+      <c r="G44" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="H44" s="17" t="s">
+      <c r="H44" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="I44" s="17" t="s">
+      <c r="I44" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="J44" s="17" t="s">
+      <c r="J44" s="16" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="45" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="16" t="n">
+    <row r="45" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="15" t="n">
         <f aca="false">B44+1</f>
         <v>25</v>
       </c>
-      <c r="C45" s="16" t="s">
+      <c r="C45" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D45" s="16" t="n">
+      <c r="D45" s="15" t="n">
         <v>6</v>
       </c>
-      <c r="F45" s="16" t="s">
+      <c r="F45" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="G45" s="16" t="s">
+      <c r="G45" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="H45" s="16" t="s">
+      <c r="H45" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="I45" s="16" t="s">
+      <c r="I45" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="J45" s="16" t="s">
+      <c r="J45" s="15" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="46" s="18" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="18" t="n">
+    <row r="46" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="17" t="n">
         <f aca="false">B45+1</f>
         <v>26</v>
       </c>
-      <c r="C46" s="18" t="s">
+      <c r="C46" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D46" s="18" t="n">
+      <c r="D46" s="17" t="n">
         <v>7</v>
       </c>
-      <c r="F46" s="18" t="s">
+      <c r="F46" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="G46" s="18" t="s">
+      <c r="G46" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="H46" s="18" t="s">
+      <c r="H46" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="I46" s="18" t="s">
+      <c r="I46" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="J46" s="18" t="s">
+      <c r="J46" s="17" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="47" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="19" t="n">
+    <row r="47" s="18" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="18" t="n">
         <f aca="false">B46+1</f>
         <v>27</v>
       </c>
-      <c r="C47" s="19" t="s">
+      <c r="C47" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D47" s="19" t="n">
+      <c r="D47" s="18" t="n">
         <v>7</v>
       </c>
-      <c r="F47" s="19" t="s">
+      <c r="F47" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="G47" s="19" t="s">
+      <c r="G47" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="H47" s="19" t="s">
+      <c r="H47" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="I47" s="19" t="s">
+      <c r="I47" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="J47" s="19" t="s">
+      <c r="J47" s="18" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="48" s="18" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="18" t="n">
+    <row r="48" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="17" t="n">
         <f aca="false">B47+1</f>
         <v>28</v>
       </c>
-      <c r="C48" s="18" t="s">
+      <c r="C48" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D48" s="18" t="n">
+      <c r="D48" s="17" t="n">
         <v>7</v>
       </c>
-      <c r="F48" s="18" t="s">
+      <c r="F48" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="G48" s="18" t="s">
+      <c r="G48" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="H48" s="18" t="s">
+      <c r="H48" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="I48" s="18" t="s">
+      <c r="I48" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="J48" s="18" t="s">
+      <c r="J48" s="17" t="s">
         <v>106</v>
       </c>
     </row>
@@ -5438,8 +5504,8 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="51.0971659919028"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="51.5222672064777"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.2105263157895"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -5455,7 +5521,7 @@
       <c r="A2" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="20" t="n">
+      <c r="B2" s="19" t="n">
         <v>43183</v>
       </c>
     </row>
@@ -5463,7 +5529,7 @@
       <c r="A3" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="20" t="n">
+      <c r="B3" s="19" t="n">
         <v>43189</v>
       </c>
     </row>
@@ -5581,7 +5647,7 @@
       <c r="F18" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="G18" s="21" t="s">
+      <c r="G18" s="20" t="s">
         <v>126</v>
       </c>
       <c r="H18" s="0" t="s">
@@ -5856,7 +5922,7 @@
       <c r="A2" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="20" t="n">
+      <c r="B2" s="19" t="n">
         <v>43192</v>
       </c>
     </row>
@@ -5864,7 +5930,7 @@
       <c r="A3" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="20" t="n">
+      <c r="B3" s="19" t="n">
         <v>43198</v>
       </c>
     </row>
@@ -6007,7 +6073,7 @@
       <c r="A2" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="20" t="n">
+      <c r="B2" s="19" t="n">
         <v>43199</v>
       </c>
     </row>
@@ -6015,7 +6081,7 @@
       <c r="A3" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="20" t="n">
+      <c r="B3" s="19" t="n">
         <v>43205</v>
       </c>
     </row>
@@ -6158,7 +6224,7 @@
       <c r="A2" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="20" t="n">
+      <c r="B2" s="19" t="n">
         <v>43206</v>
       </c>
     </row>
@@ -6166,7 +6232,7 @@
       <c r="A3" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="20" t="n">
+      <c r="B3" s="19" t="n">
         <v>43212</v>
       </c>
     </row>
@@ -6309,7 +6375,7 @@
       <c r="A2" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="20" t="n">
+      <c r="B2" s="19" t="n">
         <v>43213</v>
       </c>
     </row>
@@ -6317,7 +6383,7 @@
       <c r="A3" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="20" t="n">
+      <c r="B3" s="19" t="n">
         <v>43219</v>
       </c>
     </row>

</xml_diff>

<commit_message>
prepared files for sprint 3 submission
</commit_message>
<xml_diff>
--- a/Project/Clas Diagram and Backlog/Product Backlog.xlsx
+++ b/Project/Clas Diagram and Backlog/Product Backlog.xlsx
@@ -851,881 +851,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>Product Backlog Burn Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Product Backlog'!$B$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Left</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="5b9bd5"/>
-            </a:solidFill>
-            <a:ln w="28440">
-              <a:solidFill>
-                <a:srgbClr val="5b9bd5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="6407280">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="2067066720">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Product Backlog'!$A$8:$A$13</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Start</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Sprint 1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Sprint 2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Sprint 3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sprint 4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Sprint 5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Product Backlog'!$B$8:$B$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>22</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="95772029"/>
-        <c:axId val="18625508"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="95772029"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Sprint Number</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="18625508"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="18625508"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Features Left at End of Sprint</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="95772029"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>Product Backlog Burn Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>label 0</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Left</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="5b9bd5"/>
-            </a:solidFill>
-            <a:ln w="28440">
-              <a:solidFill>
-                <a:srgbClr val="5b9bd5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586">
-                  <a:alpha val="-17698000"/>
-                </a:srgbClr>
-              </a:solidFill>
-              <a:ln w="6407280">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln w="6022292400">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln w="6035662080">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="579d1c">
-                  <a:alpha val="-1446784704"/>
-                </a:srgbClr>
-              </a:solidFill>
-              <a:ln w="2067066720">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln w="2972724840">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="83caff">
-                  <a:alpha val="-47148408"/>
-                </a:srgbClr>
-              </a:solidFill>
-              <a:ln w="3109385880">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>categories</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Start</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Sprint 1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Sprint 2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Sprint 3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sprint 4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Sprint 5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>0</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>22</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="81013298"/>
-        <c:axId val="28930594"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="81013298"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Sprint Number</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="MM/DD/YYYY" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="28930594"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="28930594"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Features Left at End of Sprint</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="81013298"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2033,11 +1159,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="29529010"/>
-        <c:axId val="27463863"/>
+        <c:axId val="28632696"/>
+        <c:axId val="56537255"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="29529010"/>
+        <c:axId val="28632696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2111,14 +1237,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27463863"/>
+        <c:crossAx val="56537255"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="27463863"/>
+        <c:axId val="56537255"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2199,7 +1325,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29529010"/>
+        <c:crossAx val="28632696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2227,7 +1353,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2535,11 +1661,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="90499946"/>
-        <c:axId val="13907239"/>
+        <c:axId val="25782435"/>
+        <c:axId val="84568484"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="90499946"/>
+        <c:axId val="25782435"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2613,14 +1739,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13907239"/>
+        <c:crossAx val="84568484"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="13907239"/>
+        <c:axId val="84568484"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2701,7 +1827,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90499946"/>
+        <c:crossAx val="25782435"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2729,7 +1855,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3037,11 +2163,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="36143767"/>
-        <c:axId val="90113778"/>
+        <c:axId val="56593680"/>
+        <c:axId val="77296336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="36143767"/>
+        <c:axId val="56593680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3115,14 +2241,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90113778"/>
+        <c:crossAx val="77296336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90113778"/>
+        <c:axId val="77296336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3203,7 +2329,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36143767"/>
+        <c:crossAx val="56593680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3231,7 +2357,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3539,11 +2665,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="80769315"/>
-        <c:axId val="83951848"/>
+        <c:axId val="52179829"/>
+        <c:axId val="7684416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="80769315"/>
+        <c:axId val="52179829"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3617,14 +2743,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83951848"/>
+        <c:crossAx val="7684416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83951848"/>
+        <c:axId val="7684416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3705,7 +2831,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80769315"/>
+        <c:crossAx val="52179829"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3733,7 +2859,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4041,11 +3167,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="88633843"/>
-        <c:axId val="44234767"/>
+        <c:axId val="74122643"/>
+        <c:axId val="95045819"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="88633843"/>
+        <c:axId val="74122643"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4119,14 +3245,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44234767"/>
+        <c:crossAx val="95045819"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44234767"/>
+        <c:axId val="95045819"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4207,7 +3333,929 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88633843"/>
+        <c:crossAx val="74122643"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>Product Backlog Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Product Backlog'!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Left</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="5b9bd5"/>
+            </a:solidFill>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="5b9bd5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Product Backlog'!$A$8:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sprint 3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sprint 4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sprint 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Product Backlog'!$B$8:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="20040620"/>
+        <c:axId val="25703576"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="20040620"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Sprint Number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="d9d9d9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="25703576"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="25703576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Features Left at End of Sprint</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="20040620"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>Product Backlog Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>label 0</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Left</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="5b9bd5"/>
+            </a:solidFill>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="5b9bd5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sprint 3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sprint 4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sprint 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>0</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="96177975"/>
+        <c:axId val="26550505"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="96177975"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Sprint Number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="MM/DD/YYYY" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="d9d9d9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="26550505"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="26550505"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Features Left at End of Sprint</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="96177975"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4246,9 +4294,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>631080</xdr:colOff>
+      <xdr:colOff>630720</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>23760</xdr:rowOff>
+      <xdr:rowOff>23400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4256,8 +4304,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5781600" y="87480"/>
-        <a:ext cx="12251520" cy="2740320"/>
+        <a:off x="5790960" y="87480"/>
+        <a:ext cx="12327480" cy="2739960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4276,9 +4324,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>204840</xdr:colOff>
+      <xdr:colOff>204480</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>79920</xdr:rowOff>
+      <xdr:rowOff>79560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4286,8 +4334,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5724360" y="80640"/>
-        <a:ext cx="11882520" cy="2628000"/>
+        <a:off x="5733720" y="80640"/>
+        <a:ext cx="11958480" cy="2627640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4311,9 +4359,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>5040</xdr:colOff>
+      <xdr:colOff>4680</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>43200</xdr:rowOff>
+      <xdr:rowOff>42840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4322,7 +4370,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2916360" y="23040"/>
-        <a:ext cx="7813800" cy="2747880"/>
+        <a:ext cx="7860960" cy="2747520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4346,9 +4394,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>332640</xdr:colOff>
+      <xdr:colOff>332280</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>20160</xdr:rowOff>
+      <xdr:rowOff>19800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4357,7 +4405,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5636160" cy="2740320"/>
+        <a:ext cx="5635800" cy="2739960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4381,9 +4429,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>332640</xdr:colOff>
+      <xdr:colOff>332280</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>20160</xdr:rowOff>
+      <xdr:rowOff>19800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4392,7 +4440,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5636160" cy="2740320"/>
+        <a:ext cx="5635800" cy="2739960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4416,9 +4464,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>332640</xdr:colOff>
+      <xdr:colOff>332280</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>20160</xdr:rowOff>
+      <xdr:rowOff>19800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4427,7 +4475,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5636160" cy="2740320"/>
+        <a:ext cx="5635800" cy="2739960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4451,9 +4499,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>332640</xdr:colOff>
+      <xdr:colOff>332280</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>20160</xdr:rowOff>
+      <xdr:rowOff>19800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4462,7 +4510,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5636160" cy="2740320"/>
+        <a:ext cx="5635800" cy="2739960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4491,10 +4539,10 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.0688259109312"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.2064777327935"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.9554655870445"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.5263157894737"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.3805668016194"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.57085020242915"/>
@@ -4601,15 +4649,14 @@
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">C10-D11</f>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C11" s="0" t="n">
         <f aca="false">COUNT(B21:B106)</f>
         <v>28</v>
       </c>
       <c r="D11" s="1" t="n">
-        <f aca="false">D10</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E11" s="2" t="n">
         <v>43205</v>
@@ -4621,7 +4668,7 @@
       </c>
       <c r="B12" s="0" t="n">
         <f aca="false">C11-D12</f>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C12" s="0" t="n">
         <f aca="false">COUNT(B21:B107)</f>
@@ -4629,7 +4676,7 @@
       </c>
       <c r="D12" s="1" t="n">
         <f aca="false">D11</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E12" s="2" t="n">
         <v>43212</v>
@@ -4641,7 +4688,7 @@
       </c>
       <c r="B13" s="0" t="n">
         <f aca="false">C12-D13</f>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C13" s="0" t="n">
         <f aca="false">COUNT(B21:B108)</f>
@@ -4649,7 +4696,7 @@
       </c>
       <c r="D13" s="1" t="n">
         <f aca="false">D12</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E13" s="2" t="n">
         <v>43219</v>
@@ -4980,6 +5027,9 @@
       <c r="D30" s="8" t="n">
         <v>2</v>
       </c>
+      <c r="E30" s="8" t="n">
+        <v>3</v>
+      </c>
       <c r="F30" s="8" t="s">
         <v>29</v>
       </c>
@@ -5005,6 +5055,9 @@
         <v>49</v>
       </c>
       <c r="D31" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="E31" s="9" t="n">
         <v>3</v>
       </c>
       <c r="F31" s="9" t="s">
@@ -5510,8 +5563,8 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="51.5222672064777"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="51.9514170040486"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.3198380566802"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
added CSE 1325 Lecture George Rice Materials, added and7697_sprint4 for submission, added menubar
</commit_message>
<xml_diff>
--- a/Project/Clas Diagram and Backlog/Product Backlog.xlsx
+++ b/Project/Clas Diagram and Backlog/Product Backlog.xlsx
@@ -851,7 +851,929 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>Product Backlog Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Product Backlog'!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Left</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="5b9bd5"/>
+            </a:solidFill>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="5b9bd5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Product Backlog'!$A$8:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sprint 3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sprint 4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sprint 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Product Backlog'!$B$8:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="32579378"/>
+        <c:axId val="18086864"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="32579378"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Sprint Number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="d9d9d9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="18086864"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="18086864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Features Left at End of Sprint</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="32579378"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>Product Backlog Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>label 0</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Left</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="5b9bd5"/>
+            </a:solidFill>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="5b9bd5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sprint 3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sprint 4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sprint 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>0</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="38007085"/>
+        <c:axId val="79880408"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="38007085"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Sprint Number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="MM/DD/YYYY" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="d9d9d9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="79880408"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="79880408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Features Left at End of Sprint</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="38007085"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1159,11 +2081,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="28632696"/>
-        <c:axId val="56537255"/>
+        <c:axId val="60323934"/>
+        <c:axId val="78266962"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="28632696"/>
+        <c:axId val="60323934"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1237,14 +2159,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56537255"/>
+        <c:crossAx val="78266962"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="56537255"/>
+        <c:axId val="78266962"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1325,7 +2247,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28632696"/>
+        <c:crossAx val="60323934"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1353,7 +2275,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1661,11 +2583,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="25782435"/>
-        <c:axId val="84568484"/>
+        <c:axId val="75858069"/>
+        <c:axId val="78066725"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="25782435"/>
+        <c:axId val="75858069"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1739,14 +2661,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84568484"/>
+        <c:crossAx val="78066725"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84568484"/>
+        <c:axId val="78066725"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1827,7 +2749,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25782435"/>
+        <c:crossAx val="75858069"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1855,7 +2777,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2163,11 +3085,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="56593680"/>
-        <c:axId val="77296336"/>
+        <c:axId val="23507708"/>
+        <c:axId val="51729012"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="56593680"/>
+        <c:axId val="23507708"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2241,14 +3163,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77296336"/>
+        <c:crossAx val="51729012"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77296336"/>
+        <c:axId val="51729012"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2329,7 +3251,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56593680"/>
+        <c:crossAx val="23507708"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2357,7 +3279,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2665,11 +3587,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="52179829"/>
-        <c:axId val="7684416"/>
+        <c:axId val="9765341"/>
+        <c:axId val="46338758"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="52179829"/>
+        <c:axId val="9765341"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2743,14 +3665,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7684416"/>
+        <c:crossAx val="46338758"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="7684416"/>
+        <c:axId val="46338758"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2831,7 +3753,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52179829"/>
+        <c:crossAx val="9765341"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2859,7 +3781,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3167,11 +4089,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="74122643"/>
-        <c:axId val="95045819"/>
+        <c:axId val="4756767"/>
+        <c:axId val="47255395"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="74122643"/>
+        <c:axId val="4756767"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3245,14 +4167,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95045819"/>
+        <c:crossAx val="47255395"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95045819"/>
+        <c:axId val="47255395"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3333,929 +4255,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74122643"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>Product Backlog Burn Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Product Backlog'!$B$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Left</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="5b9bd5"/>
-            </a:solidFill>
-            <a:ln w="28440">
-              <a:solidFill>
-                <a:srgbClr val="5b9bd5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="6407280">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="2067066720">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Product Backlog'!$A$8:$A$13</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Start</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Sprint 1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Sprint 2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Sprint 3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sprint 4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Sprint 5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Product Backlog'!$B$8:$B$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>20</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="20040620"/>
-        <c:axId val="25703576"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="20040620"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Sprint Number</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="25703576"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="25703576"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Features Left at End of Sprint</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="20040620"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>Product Backlog Burn Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>label 0</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Left</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="5b9bd5"/>
-            </a:solidFill>
-            <a:ln w="28440">
-              <a:solidFill>
-                <a:srgbClr val="5b9bd5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="6407280">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="2067066720">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>categories</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Start</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Sprint 1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Sprint 2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Sprint 3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sprint 4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Sprint 5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>0</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>22</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="96177975"/>
-        <c:axId val="26550505"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="96177975"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Sprint Number</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="MM/DD/YYYY" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="26550505"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="26550505"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Features Left at End of Sprint</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="96177975"/>
+        <c:crossAx val="4756767"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4294,9 +4294,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>630720</xdr:colOff>
+      <xdr:colOff>630360</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>23400</xdr:rowOff>
+      <xdr:rowOff>23040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4304,8 +4304,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5790960" y="87480"/>
-        <a:ext cx="12327480" cy="2739960"/>
+        <a:off x="5800680" y="87480"/>
+        <a:ext cx="12393720" cy="2739600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4324,9 +4324,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>204480</xdr:colOff>
+      <xdr:colOff>204120</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>79560</xdr:rowOff>
+      <xdr:rowOff>79200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4334,8 +4334,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5733720" y="80640"/>
-        <a:ext cx="11958480" cy="2627640"/>
+        <a:off x="5743440" y="80640"/>
+        <a:ext cx="12024720" cy="2627280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4359,9 +4359,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>4680</xdr:colOff>
+      <xdr:colOff>4320</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>42840</xdr:rowOff>
+      <xdr:rowOff>42480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4370,7 +4370,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2916360" y="23040"/>
-        <a:ext cx="7860960" cy="2747520"/>
+        <a:ext cx="7908120" cy="2747160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4394,9 +4394,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>332280</xdr:colOff>
+      <xdr:colOff>331920</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>19800</xdr:rowOff>
+      <xdr:rowOff>19440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4405,7 +4405,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5635800" cy="2739960"/>
+        <a:ext cx="5635440" cy="2739600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4429,9 +4429,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>332280</xdr:colOff>
+      <xdr:colOff>331920</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>19800</xdr:rowOff>
+      <xdr:rowOff>19440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4440,7 +4440,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5635800" cy="2739960"/>
+        <a:ext cx="5635440" cy="2739600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4464,9 +4464,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>332280</xdr:colOff>
+      <xdr:colOff>331920</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>19800</xdr:rowOff>
+      <xdr:rowOff>19440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4475,7 +4475,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5635800" cy="2739960"/>
+        <a:ext cx="5635440" cy="2739600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4499,9 +4499,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>332280</xdr:colOff>
+      <xdr:colOff>331920</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>19800</xdr:rowOff>
+      <xdr:rowOff>19440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4510,7 +4510,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5635800" cy="2739960"/>
+        <a:ext cx="5635440" cy="2739600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4530,8 +4530,8 @@
   </sheetPr>
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E38" activeCellId="0" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -4539,10 +4539,10 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.1781376518219"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.5263157894737"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.3805668016194"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.8502024291498"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.7044534412956"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.57085020242915"/>
@@ -4668,15 +4668,14 @@
       </c>
       <c r="B12" s="0" t="n">
         <f aca="false">C11-D12</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C12" s="0" t="n">
         <f aca="false">COUNT(B21:B107)</f>
         <v>28</v>
       </c>
       <c r="D12" s="1" t="n">
-        <f aca="false">D11</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E12" s="2" t="n">
         <v>43212</v>
@@ -4688,7 +4687,7 @@
       </c>
       <c r="B13" s="0" t="n">
         <f aca="false">C12-D13</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C13" s="0" t="n">
         <f aca="false">COUNT(B21:B108)</f>
@@ -4696,7 +4695,7 @@
       </c>
       <c r="D13" s="1" t="n">
         <f aca="false">D12</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E13" s="2" t="n">
         <v>43219</v>
@@ -5087,6 +5086,9 @@
       <c r="D32" s="10" t="n">
         <v>3</v>
       </c>
+      <c r="E32" s="10" t="n">
+        <v>4</v>
+      </c>
       <c r="F32" s="10" t="s">
         <v>29</v>
       </c>
@@ -5114,6 +5116,9 @@
       <c r="D33" s="9" t="n">
         <v>3</v>
       </c>
+      <c r="E33" s="9" t="n">
+        <v>4</v>
+      </c>
       <c r="F33" s="9" t="s">
         <v>42</v>
       </c>
@@ -5141,6 +5146,9 @@
       <c r="D34" s="11" t="n">
         <v>4</v>
       </c>
+      <c r="E34" s="11" t="n">
+        <v>4</v>
+      </c>
       <c r="F34" s="11" t="s">
         <v>29</v>
       </c>
@@ -5168,6 +5176,9 @@
       <c r="D35" s="12" t="n">
         <v>4</v>
       </c>
+      <c r="E35" s="12" t="n">
+        <v>4</v>
+      </c>
       <c r="F35" s="12" t="s">
         <v>39</v>
       </c>
@@ -5274,6 +5285,9 @@
         <v>49</v>
       </c>
       <c r="D39" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="E39" s="12" t="n">
         <v>4</v>
       </c>
       <c r="F39" s="12" t="s">
@@ -5563,8 +5577,8 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="51.9514170040486"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="52.3805668016194"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
working on adding checked_out_list
</commit_message>
<xml_diff>
--- a/Project/Clas Diagram and Backlog/Product Backlog.xlsx
+++ b/Project/Clas Diagram and Backlog/Product Backlog.xlsx
@@ -851,929 +851,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>Product Backlog Burn Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Product Backlog'!$B$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Left</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="5b9bd5"/>
-            </a:solidFill>
-            <a:ln w="28440">
-              <a:solidFill>
-                <a:srgbClr val="5b9bd5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="6407280">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="2067066720">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Product Backlog'!$A$8:$A$13</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Start</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Sprint 1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Sprint 2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Sprint 3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sprint 4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Sprint 5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Product Backlog'!$B$8:$B$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>15</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="32579378"/>
-        <c:axId val="18086864"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="32579378"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Sprint Number</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="18086864"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="18086864"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Features Left at End of Sprint</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="32579378"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>Product Backlog Burn Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>label 0</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Left</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="5b9bd5"/>
-            </a:solidFill>
-            <a:ln w="28440">
-              <a:solidFill>
-                <a:srgbClr val="5b9bd5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="6407280">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="2067066720">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>categories</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Start</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Sprint 1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Sprint 2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Sprint 3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sprint 4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Sprint 5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>0</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>22</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="38007085"/>
-        <c:axId val="79880408"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="38007085"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Sprint Number</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="MM/DD/YYYY" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="79880408"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="79880408"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Features Left at End of Sprint</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="38007085"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2081,11 +1159,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="60323934"/>
-        <c:axId val="78266962"/>
+        <c:axId val="29078998"/>
+        <c:axId val="84046838"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="60323934"/>
+        <c:axId val="29078998"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2159,14 +1237,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78266962"/>
+        <c:crossAx val="84046838"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78266962"/>
+        <c:axId val="84046838"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2247,7 +1325,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60323934"/>
+        <c:crossAx val="29078998"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2275,7 +1353,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2583,11 +1661,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="75858069"/>
-        <c:axId val="78066725"/>
+        <c:axId val="26263227"/>
+        <c:axId val="41527921"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="75858069"/>
+        <c:axId val="26263227"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2661,14 +1739,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78066725"/>
+        <c:crossAx val="41527921"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78066725"/>
+        <c:axId val="41527921"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2749,7 +1827,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75858069"/>
+        <c:crossAx val="26263227"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2777,7 +1855,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3085,11 +2163,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="23507708"/>
-        <c:axId val="51729012"/>
+        <c:axId val="64693547"/>
+        <c:axId val="92460705"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="23507708"/>
+        <c:axId val="64693547"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3163,14 +2241,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51729012"/>
+        <c:crossAx val="92460705"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51729012"/>
+        <c:axId val="92460705"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3251,7 +2329,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23507708"/>
+        <c:crossAx val="64693547"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3279,7 +2357,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3587,11 +2665,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="9765341"/>
-        <c:axId val="46338758"/>
+        <c:axId val="92579094"/>
+        <c:axId val="38458284"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="9765341"/>
+        <c:axId val="92579094"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3665,14 +2743,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46338758"/>
+        <c:crossAx val="38458284"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46338758"/>
+        <c:axId val="38458284"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3753,7 +2831,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9765341"/>
+        <c:crossAx val="92579094"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3781,7 +2859,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4089,11 +3167,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="4756767"/>
-        <c:axId val="47255395"/>
+        <c:axId val="89383797"/>
+        <c:axId val="74415128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="4756767"/>
+        <c:axId val="89383797"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4167,14 +3245,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47255395"/>
+        <c:crossAx val="74415128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47255395"/>
+        <c:axId val="74415128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4255,7 +3333,929 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4756767"/>
+        <c:crossAx val="89383797"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>Product Backlog Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Product Backlog'!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Left</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="5b9bd5"/>
+            </a:solidFill>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="5b9bd5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Product Backlog'!$A$8:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sprint 3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sprint 4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sprint 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Product Backlog'!$B$8:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="28286693"/>
+        <c:axId val="90033347"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="28286693"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Sprint Number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="d9d9d9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="90033347"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="90033347"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Features Left at End of Sprint</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="28286693"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>Product Backlog Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>label 0</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Left</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="5b9bd5"/>
+            </a:solidFill>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="5b9bd5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sprint 3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sprint 4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sprint 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>0</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="56085650"/>
+        <c:axId val="44603541"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="56085650"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Sprint Number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="MM/DD/YYYY" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="d9d9d9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="44603541"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="44603541"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Features Left at End of Sprint</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="56085650"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4294,9 +4294,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>630360</xdr:colOff>
+      <xdr:colOff>630000</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>23040</xdr:rowOff>
+      <xdr:rowOff>22680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4304,8 +4304,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5800680" y="87480"/>
-        <a:ext cx="12393720" cy="2739600"/>
+        <a:off x="5810040" y="87480"/>
+        <a:ext cx="12459960" cy="2739240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4324,9 +4324,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>204120</xdr:colOff>
+      <xdr:colOff>203760</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>79200</xdr:rowOff>
+      <xdr:rowOff>78840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4334,8 +4334,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5743440" y="80640"/>
-        <a:ext cx="12024720" cy="2627280"/>
+        <a:off x="5752800" y="80640"/>
+        <a:ext cx="12090960" cy="2626920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4359,9 +4359,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>4320</xdr:colOff>
+      <xdr:colOff>3960</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>42480</xdr:rowOff>
+      <xdr:rowOff>42120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4370,7 +4370,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2916360" y="23040"/>
-        <a:ext cx="7908120" cy="2747160"/>
+        <a:ext cx="7955280" cy="2746800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4394,9 +4394,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>331920</xdr:colOff>
+      <xdr:colOff>331560</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>19440</xdr:rowOff>
+      <xdr:rowOff>19080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4405,7 +4405,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5635440" cy="2739600"/>
+        <a:ext cx="5635080" cy="2739240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4429,9 +4429,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>331920</xdr:colOff>
+      <xdr:colOff>331560</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>19440</xdr:rowOff>
+      <xdr:rowOff>19080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4440,7 +4440,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5635440" cy="2739600"/>
+        <a:ext cx="5635080" cy="2739240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4464,9 +4464,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>331920</xdr:colOff>
+      <xdr:colOff>331560</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>19440</xdr:rowOff>
+      <xdr:rowOff>19080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4475,7 +4475,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5635440" cy="2739600"/>
+        <a:ext cx="5635080" cy="2739240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4499,9 +4499,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>331920</xdr:colOff>
+      <xdr:colOff>331560</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>19440</xdr:rowOff>
+      <xdr:rowOff>19080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4510,7 +4510,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5635440" cy="2739600"/>
+        <a:ext cx="5635080" cy="2739240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4530,8 +4530,8 @@
   </sheetPr>
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E38" activeCellId="0" sqref="E38"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -4539,10 +4539,10 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.8502024291498"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.7044534412956"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.17004048583"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.0242914979757"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.57085020242915"/>
@@ -4668,14 +4668,14 @@
       </c>
       <c r="B12" s="0" t="n">
         <f aca="false">C11-D12</f>
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C12" s="0" t="n">
         <f aca="false">COUNT(B21:B107)</f>
         <v>28</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E12" s="2" t="n">
         <v>43212</v>
@@ -4687,7 +4687,7 @@
       </c>
       <c r="B13" s="0" t="n">
         <f aca="false">C12-D13</f>
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C13" s="0" t="n">
         <f aca="false">COUNT(B21:B108)</f>
@@ -4695,7 +4695,7 @@
       </c>
       <c r="D13" s="1" t="n">
         <f aca="false">D12</f>
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E13" s="2" t="n">
         <v>43219</v>
@@ -4945,6 +4945,9 @@
       <c r="D27" s="7" t="n">
         <v>2</v>
       </c>
+      <c r="E27" s="7" t="n">
+        <v>4</v>
+      </c>
       <c r="F27" s="7" t="s">
         <v>39</v>
       </c>
@@ -4972,6 +4975,9 @@
       <c r="D28" s="8" t="n">
         <v>2</v>
       </c>
+      <c r="E28" s="8" t="n">
+        <v>4</v>
+      </c>
       <c r="F28" s="8" t="s">
         <v>39</v>
       </c>
@@ -4999,6 +5005,9 @@
       <c r="D29" s="7" t="n">
         <v>2</v>
       </c>
+      <c r="E29" s="7" t="n">
+        <v>4</v>
+      </c>
       <c r="F29" s="7" t="s">
         <v>42</v>
       </c>
@@ -5206,6 +5215,9 @@
       <c r="D36" s="11" t="n">
         <v>4</v>
       </c>
+      <c r="E36" s="11" t="n">
+        <v>4</v>
+      </c>
       <c r="F36" s="11" t="s">
         <v>39</v>
       </c>
@@ -5233,6 +5245,9 @@
       <c r="D37" s="12" t="n">
         <v>4</v>
       </c>
+      <c r="E37" s="12" t="n">
+        <v>4</v>
+      </c>
       <c r="F37" s="12" t="s">
         <v>39</v>
       </c>
@@ -5260,6 +5275,9 @@
       <c r="D38" s="11" t="n">
         <v>4</v>
       </c>
+      <c r="E38" s="11" t="n">
+        <v>4</v>
+      </c>
       <c r="F38" s="11" t="s">
         <v>42</v>
       </c>
@@ -5344,6 +5362,9 @@
       <c r="D41" s="14" t="n">
         <v>5</v>
       </c>
+      <c r="E41" s="14" t="n">
+        <v>4</v>
+      </c>
       <c r="F41" s="14" t="s">
         <v>29</v>
       </c>
@@ -5370,6 +5391,9 @@
       </c>
       <c r="D42" s="13" t="n">
         <v>5</v>
+      </c>
+      <c r="E42" s="13" t="n">
+        <v>4</v>
       </c>
       <c r="F42" s="13" t="s">
         <v>29</v>
@@ -5577,8 +5601,8 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="52.3805668016194"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="52.8097165991903"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
updated product backlog, class diagram, and all the files for and7697_sprint4 submission
</commit_message>
<xml_diff>
--- a/Project/Clas Diagram and Backlog/Product Backlog.xlsx
+++ b/Project/Clas Diagram and Backlog/Product Backlog.xlsx
@@ -851,7 +851,929 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>Product Backlog Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Product Backlog'!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Left</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="5b9bd5"/>
+            </a:solidFill>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="5b9bd5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Product Backlog'!$A$8:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sprint 3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sprint 4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sprint 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Product Backlog'!$B$8:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="11451979"/>
+        <c:axId val="51323233"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="11451979"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Sprint Number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="d9d9d9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="51323233"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="51323233"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Features Left at End of Sprint</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="11451979"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>Product Backlog Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>label 0</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Left</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="5b9bd5"/>
+            </a:solidFill>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="5b9bd5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sprint 3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sprint 4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sprint 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>0</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="41110457"/>
+        <c:axId val="80834475"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="41110457"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Sprint Number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="MM/DD/YYYY" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="d9d9d9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="80834475"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="80834475"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Features Left at End of Sprint</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="41110457"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1159,11 +2081,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="29078998"/>
-        <c:axId val="84046838"/>
+        <c:axId val="41685327"/>
+        <c:axId val="93951082"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="29078998"/>
+        <c:axId val="41685327"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1237,14 +2159,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84046838"/>
+        <c:crossAx val="93951082"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84046838"/>
+        <c:axId val="93951082"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1325,7 +2247,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29078998"/>
+        <c:crossAx val="41685327"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1353,7 +2275,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1661,11 +2583,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="26263227"/>
-        <c:axId val="41527921"/>
+        <c:axId val="10276606"/>
+        <c:axId val="13094713"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="26263227"/>
+        <c:axId val="10276606"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1739,14 +2661,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41527921"/>
+        <c:crossAx val="13094713"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41527921"/>
+        <c:axId val="13094713"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1827,7 +2749,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26263227"/>
+        <c:crossAx val="10276606"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1855,7 +2777,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2163,11 +3085,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="64693547"/>
-        <c:axId val="92460705"/>
+        <c:axId val="6998720"/>
+        <c:axId val="96614155"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="64693547"/>
+        <c:axId val="6998720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2241,14 +3163,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92460705"/>
+        <c:crossAx val="96614155"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92460705"/>
+        <c:axId val="96614155"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2329,7 +3251,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64693547"/>
+        <c:crossAx val="6998720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2357,7 +3279,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2665,11 +3587,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="92579094"/>
-        <c:axId val="38458284"/>
+        <c:axId val="19080758"/>
+        <c:axId val="22134406"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="92579094"/>
+        <c:axId val="19080758"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2743,14 +3665,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38458284"/>
+        <c:crossAx val="22134406"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="38458284"/>
+        <c:axId val="22134406"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2831,7 +3753,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92579094"/>
+        <c:crossAx val="19080758"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2859,7 +3781,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3167,11 +4089,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="89383797"/>
-        <c:axId val="74415128"/>
+        <c:axId val="94711907"/>
+        <c:axId val="71930026"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="89383797"/>
+        <c:axId val="94711907"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3245,14 +4167,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74415128"/>
+        <c:crossAx val="71930026"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74415128"/>
+        <c:axId val="71930026"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3333,929 +4255,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89383797"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>Product Backlog Burn Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Product Backlog'!$B$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Left</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="5b9bd5"/>
-            </a:solidFill>
-            <a:ln w="28440">
-              <a:solidFill>
-                <a:srgbClr val="5b9bd5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="6407280">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="2067066720">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Product Backlog'!$A$8:$A$13</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Start</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Sprint 1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Sprint 2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Sprint 3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sprint 4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Sprint 5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Product Backlog'!$B$8:$B$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="28286693"/>
-        <c:axId val="90033347"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="28286693"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Sprint Number</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="90033347"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="90033347"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Features Left at End of Sprint</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="28286693"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>Product Backlog Burn Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>label 0</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Left</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="5b9bd5"/>
-            </a:solidFill>
-            <a:ln w="28440">
-              <a:solidFill>
-                <a:srgbClr val="5b9bd5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="6407280">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="2067066720">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>categories</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Start</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Sprint 1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Sprint 2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Sprint 3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sprint 4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Sprint 5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>0</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>22</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="56085650"/>
-        <c:axId val="44603541"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="56085650"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Sprint Number</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="MM/DD/YYYY" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="44603541"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="44603541"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Features Left at End of Sprint</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="56085650"/>
+        <c:crossAx val="94711907"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4530,8 +4530,8 @@
   </sheetPr>
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E40" activeCellId="0" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>

<commit_message>
check_in() and check_out() tested and works perfectly
</commit_message>
<xml_diff>
--- a/Project/Clas Diagram and Backlog/Product Backlog.xlsx
+++ b/Project/Clas Diagram and Backlog/Product Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" state="visible" r:id="rId2"/>
@@ -851,929 +851,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>Product Backlog Burn Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Product Backlog'!$B$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Left</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="5b9bd5"/>
-            </a:solidFill>
-            <a:ln w="28440">
-              <a:solidFill>
-                <a:srgbClr val="5b9bd5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="6407280">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="2067066720">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Product Backlog'!$A$8:$A$13</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Start</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Sprint 1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Sprint 2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Sprint 3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sprint 4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Sprint 5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Product Backlog'!$B$8:$B$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="11451979"/>
-        <c:axId val="51323233"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="11451979"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Sprint Number</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="51323233"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="51323233"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Features Left at End of Sprint</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="11451979"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>Product Backlog Burn Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>label 0</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Left</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="5b9bd5"/>
-            </a:solidFill>
-            <a:ln w="28440">
-              <a:solidFill>
-                <a:srgbClr val="5b9bd5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="6407280">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="2067066720">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>categories</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Start</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Sprint 1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Sprint 2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Sprint 3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sprint 4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Sprint 5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>0</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>22</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="41110457"/>
-        <c:axId val="80834475"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="41110457"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Sprint Number</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="MM/DD/YYYY" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="80834475"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="80834475"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Features Left at End of Sprint</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="41110457"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2081,11 +1159,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="41685327"/>
-        <c:axId val="93951082"/>
+        <c:axId val="49361713"/>
+        <c:axId val="58393359"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="41685327"/>
+        <c:axId val="49361713"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2159,14 +1237,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93951082"/>
+        <c:crossAx val="58393359"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93951082"/>
+        <c:axId val="58393359"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2247,7 +1325,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41685327"/>
+        <c:crossAx val="49361713"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2275,7 +1353,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2583,11 +1661,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="10276606"/>
-        <c:axId val="13094713"/>
+        <c:axId val="40309888"/>
+        <c:axId val="60067954"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="10276606"/>
+        <c:axId val="40309888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2661,14 +1739,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13094713"/>
+        <c:crossAx val="60067954"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="13094713"/>
+        <c:axId val="60067954"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2749,7 +1827,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10276606"/>
+        <c:crossAx val="40309888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2777,7 +1855,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3085,11 +2163,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="6998720"/>
-        <c:axId val="96614155"/>
+        <c:axId val="64891630"/>
+        <c:axId val="78155265"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="6998720"/>
+        <c:axId val="64891630"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3163,14 +2241,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96614155"/>
+        <c:crossAx val="78155265"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96614155"/>
+        <c:axId val="78155265"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3251,7 +2329,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6998720"/>
+        <c:crossAx val="64891630"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3279,7 +2357,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3587,11 +2665,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="19080758"/>
-        <c:axId val="22134406"/>
+        <c:axId val="81186570"/>
+        <c:axId val="38208509"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="19080758"/>
+        <c:axId val="81186570"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3665,14 +2743,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22134406"/>
+        <c:crossAx val="38208509"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="22134406"/>
+        <c:axId val="38208509"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3753,7 +2831,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19080758"/>
+        <c:crossAx val="81186570"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3781,7 +2859,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4089,11 +3167,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="94711907"/>
-        <c:axId val="71930026"/>
+        <c:axId val="66886927"/>
+        <c:axId val="69166363"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="94711907"/>
+        <c:axId val="66886927"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4167,14 +3245,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71930026"/>
+        <c:crossAx val="69166363"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71930026"/>
+        <c:axId val="69166363"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4255,7 +3333,929 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94711907"/>
+        <c:crossAx val="66886927"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>Product Backlog Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Product Backlog'!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Left</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="5b9bd5"/>
+            </a:solidFill>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="5b9bd5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Product Backlog'!$A$8:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sprint 3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sprint 4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sprint 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Product Backlog'!$B$8:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="30581476"/>
+        <c:axId val="68919555"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="30581476"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Sprint Number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="d9d9d9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="68919555"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="68919555"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Features Left at End of Sprint</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="30581476"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>Product Backlog Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>label 0</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Left</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="5b9bd5"/>
+            </a:solidFill>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="5b9bd5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sprint 3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sprint 4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sprint 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>0</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="81362879"/>
+        <c:axId val="87093365"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="81362879"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Sprint Number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="MM/DD/YYYY" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="d9d9d9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="87093365"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="87093365"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Features Left at End of Sprint</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="81362879"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4294,9 +4294,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>630000</xdr:colOff>
+      <xdr:colOff>629640</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>22680</xdr:rowOff>
+      <xdr:rowOff>22320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4304,8 +4304,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5810040" y="87480"/>
-        <a:ext cx="12459960" cy="2739240"/>
+        <a:off x="5819760" y="87480"/>
+        <a:ext cx="12526200" cy="2738880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4324,9 +4324,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>203760</xdr:colOff>
+      <xdr:colOff>203400</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>78840</xdr:rowOff>
+      <xdr:rowOff>78480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4334,8 +4334,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5752800" y="80640"/>
-        <a:ext cx="12090960" cy="2626920"/>
+        <a:off x="5762520" y="80640"/>
+        <a:ext cx="12157200" cy="2626560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4359,9 +4359,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>3960</xdr:colOff>
+      <xdr:colOff>3600</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>42120</xdr:rowOff>
+      <xdr:rowOff>41760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4370,7 +4370,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2916360" y="23040"/>
-        <a:ext cx="7955280" cy="2746800"/>
+        <a:ext cx="8002800" cy="2746440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4394,9 +4394,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>331560</xdr:colOff>
+      <xdr:colOff>331200</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>19080</xdr:rowOff>
+      <xdr:rowOff>18720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4405,7 +4405,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5635080" cy="2739240"/>
+        <a:ext cx="5634720" cy="2738880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4429,9 +4429,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>331560</xdr:colOff>
+      <xdr:colOff>331200</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>19080</xdr:rowOff>
+      <xdr:rowOff>18720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4440,7 +4440,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5635080" cy="2739240"/>
+        <a:ext cx="5634720" cy="2738880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4464,9 +4464,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>331560</xdr:colOff>
+      <xdr:colOff>331200</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>19080</xdr:rowOff>
+      <xdr:rowOff>18720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4475,7 +4475,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5635080" cy="2739240"/>
+        <a:ext cx="5634720" cy="2738880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4499,9 +4499,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>331560</xdr:colOff>
+      <xdr:colOff>331200</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>19080</xdr:rowOff>
+      <xdr:rowOff>18720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4510,7 +4510,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5635080" cy="2739240"/>
+        <a:ext cx="5634720" cy="2738880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4530,7 +4530,7 @@
   </sheetPr>
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E40" activeCellId="0" sqref="E40"/>
     </sheetView>
   </sheetViews>
@@ -4539,10 +4539,10 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.17004048583"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.0242914979757"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.5991902834008"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.3481781376518"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.57085020242915"/>
@@ -4668,14 +4668,14 @@
       </c>
       <c r="B12" s="0" t="n">
         <f aca="false">C11-D12</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="0" t="n">
         <f aca="false">COUNT(B21:B107)</f>
         <v>28</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E12" s="2" t="n">
         <v>43212</v>
@@ -4687,7 +4687,7 @@
       </c>
       <c r="B13" s="0" t="n">
         <f aca="false">C12-D13</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" s="0" t="n">
         <f aca="false">COUNT(B21:B108)</f>
@@ -4695,7 +4695,7 @@
       </c>
       <c r="D13" s="1" t="n">
         <f aca="false">D12</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E13" s="2" t="n">
         <v>43219</v>
@@ -5334,6 +5334,9 @@
       </c>
       <c r="D40" s="13" t="n">
         <v>5</v>
+      </c>
+      <c r="E40" s="13" t="n">
+        <v>4</v>
       </c>
       <c r="F40" s="13" t="s">
         <v>29</v>
@@ -5601,8 +5604,8 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="52.8097165991903"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="53.2388663967611"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
check_in() and check_out() tested and works perfectly, prepared product backlog, class diagram, and and7697_sprint4 for Blackboard submission
</commit_message>
<xml_diff>
--- a/Project/Clas Diagram and Backlog/Product Backlog.xlsx
+++ b/Project/Clas Diagram and Backlog/Product Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" state="visible" r:id="rId2"/>
@@ -851,929 +851,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>Product Backlog Burn Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Product Backlog'!$B$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Left</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="5b9bd5"/>
-            </a:solidFill>
-            <a:ln w="28440">
-              <a:solidFill>
-                <a:srgbClr val="5b9bd5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="6407280">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="2067066720">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Product Backlog'!$A$8:$A$13</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Start</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Sprint 1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Sprint 2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Sprint 3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sprint 4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Sprint 5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Product Backlog'!$B$8:$B$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="11451979"/>
-        <c:axId val="51323233"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="11451979"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Sprint Number</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="51323233"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="51323233"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Features Left at End of Sprint</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="11451979"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>Product Backlog Burn Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>label 0</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Left</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="5b9bd5"/>
-            </a:solidFill>
-            <a:ln w="28440">
-              <a:solidFill>
-                <a:srgbClr val="5b9bd5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="6407280">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="2067066720">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>categories</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Start</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Sprint 1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Sprint 2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Sprint 3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sprint 4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Sprint 5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>0</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>22</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="41110457"/>
-        <c:axId val="80834475"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="41110457"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Sprint Number</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="MM/DD/YYYY" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="80834475"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="80834475"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Features Left at End of Sprint</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="41110457"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2081,11 +1159,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="41685327"/>
-        <c:axId val="93951082"/>
+        <c:axId val="49361713"/>
+        <c:axId val="58393359"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="41685327"/>
+        <c:axId val="49361713"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2159,14 +1237,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93951082"/>
+        <c:crossAx val="58393359"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93951082"/>
+        <c:axId val="58393359"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2247,7 +1325,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41685327"/>
+        <c:crossAx val="49361713"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2275,7 +1353,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2583,11 +1661,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="10276606"/>
-        <c:axId val="13094713"/>
+        <c:axId val="40309888"/>
+        <c:axId val="60067954"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="10276606"/>
+        <c:axId val="40309888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2661,14 +1739,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13094713"/>
+        <c:crossAx val="60067954"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="13094713"/>
+        <c:axId val="60067954"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2749,7 +1827,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10276606"/>
+        <c:crossAx val="40309888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2777,7 +1855,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3085,11 +2163,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="6998720"/>
-        <c:axId val="96614155"/>
+        <c:axId val="64891630"/>
+        <c:axId val="78155265"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="6998720"/>
+        <c:axId val="64891630"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3163,14 +2241,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96614155"/>
+        <c:crossAx val="78155265"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96614155"/>
+        <c:axId val="78155265"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3251,7 +2329,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6998720"/>
+        <c:crossAx val="64891630"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3279,7 +2357,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3587,11 +2665,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="19080758"/>
-        <c:axId val="22134406"/>
+        <c:axId val="81186570"/>
+        <c:axId val="38208509"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="19080758"/>
+        <c:axId val="81186570"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3665,14 +2743,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22134406"/>
+        <c:crossAx val="38208509"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="22134406"/>
+        <c:axId val="38208509"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3753,7 +2831,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19080758"/>
+        <c:crossAx val="81186570"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3781,7 +2859,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4089,11 +3167,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="94711907"/>
-        <c:axId val="71930026"/>
+        <c:axId val="66886927"/>
+        <c:axId val="69166363"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="94711907"/>
+        <c:axId val="66886927"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4167,14 +3245,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71930026"/>
+        <c:crossAx val="69166363"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71930026"/>
+        <c:axId val="69166363"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4255,7 +3333,929 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94711907"/>
+        <c:crossAx val="66886927"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>Product Backlog Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Product Backlog'!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Left</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="5b9bd5"/>
+            </a:solidFill>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="5b9bd5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Product Backlog'!$A$8:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sprint 3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sprint 4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sprint 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Product Backlog'!$B$8:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="30581476"/>
+        <c:axId val="68919555"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="30581476"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Sprint Number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="d9d9d9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="68919555"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="68919555"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Features Left at End of Sprint</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="30581476"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>Product Backlog Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>label 0</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Left</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="5b9bd5"/>
+            </a:solidFill>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="5b9bd5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sprint 3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sprint 4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sprint 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>0</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="81362879"/>
+        <c:axId val="87093365"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="81362879"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Sprint Number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="MM/DD/YYYY" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="d9d9d9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="87093365"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="87093365"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Features Left at End of Sprint</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="81362879"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4294,9 +4294,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>630000</xdr:colOff>
+      <xdr:colOff>629640</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>22680</xdr:rowOff>
+      <xdr:rowOff>22320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4304,8 +4304,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5810040" y="87480"/>
-        <a:ext cx="12459960" cy="2739240"/>
+        <a:off x="5819760" y="87480"/>
+        <a:ext cx="12526200" cy="2738880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4324,9 +4324,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>203760</xdr:colOff>
+      <xdr:colOff>203400</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>78840</xdr:rowOff>
+      <xdr:rowOff>78480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4334,8 +4334,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5752800" y="80640"/>
-        <a:ext cx="12090960" cy="2626920"/>
+        <a:off x="5762520" y="80640"/>
+        <a:ext cx="12157200" cy="2626560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4359,9 +4359,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>3960</xdr:colOff>
+      <xdr:colOff>3600</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>42120</xdr:rowOff>
+      <xdr:rowOff>41760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4370,7 +4370,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2916360" y="23040"/>
-        <a:ext cx="7955280" cy="2746800"/>
+        <a:ext cx="8002800" cy="2746440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4394,9 +4394,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>331560</xdr:colOff>
+      <xdr:colOff>331200</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>19080</xdr:rowOff>
+      <xdr:rowOff>18720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4405,7 +4405,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5635080" cy="2739240"/>
+        <a:ext cx="5634720" cy="2738880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4429,9 +4429,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>331560</xdr:colOff>
+      <xdr:colOff>331200</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>19080</xdr:rowOff>
+      <xdr:rowOff>18720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4440,7 +4440,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5635080" cy="2739240"/>
+        <a:ext cx="5634720" cy="2738880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4464,9 +4464,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>331560</xdr:colOff>
+      <xdr:colOff>331200</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>19080</xdr:rowOff>
+      <xdr:rowOff>18720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4475,7 +4475,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5635080" cy="2739240"/>
+        <a:ext cx="5634720" cy="2738880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4499,9 +4499,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>331560</xdr:colOff>
+      <xdr:colOff>331200</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>19080</xdr:rowOff>
+      <xdr:rowOff>18720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4510,7 +4510,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5635080" cy="2739240"/>
+        <a:ext cx="5634720" cy="2738880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4530,7 +4530,7 @@
   </sheetPr>
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E40" activeCellId="0" sqref="E40"/>
     </sheetView>
   </sheetViews>
@@ -4539,10 +4539,10 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.17004048583"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.0242914979757"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.5991902834008"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.3481781376518"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.57085020242915"/>
@@ -4668,14 +4668,14 @@
       </c>
       <c r="B12" s="0" t="n">
         <f aca="false">C11-D12</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="0" t="n">
         <f aca="false">COUNT(B21:B107)</f>
         <v>28</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E12" s="2" t="n">
         <v>43212</v>
@@ -4687,7 +4687,7 @@
       </c>
       <c r="B13" s="0" t="n">
         <f aca="false">C12-D13</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" s="0" t="n">
         <f aca="false">COUNT(B21:B108)</f>
@@ -4695,7 +4695,7 @@
       </c>
       <c r="D13" s="1" t="n">
         <f aca="false">D12</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E13" s="2" t="n">
         <v>43219</v>
@@ -5334,6 +5334,9 @@
       </c>
       <c r="D40" s="13" t="n">
         <v>5</v>
+      </c>
+      <c r="E40" s="13" t="n">
+        <v>4</v>
       </c>
       <c r="F40" s="13" t="s">
         <v>29</v>
@@ -5601,8 +5604,8 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="52.8097165991903"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="53.2388663967611"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
updated product backlog and class diagram, little progress on load in library class
</commit_message>
<xml_diff>
--- a/Project/Clas Diagram and Backlog/Product Backlog.xlsx
+++ b/Project/Clas Diagram and Backlog/Product Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" state="visible" r:id="rId2"/>
@@ -1159,11 +1159,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="49361713"/>
-        <c:axId val="58393359"/>
+        <c:axId val="31811527"/>
+        <c:axId val="68280613"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="49361713"/>
+        <c:axId val="31811527"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1237,14 +1237,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58393359"/>
+        <c:crossAx val="68280613"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58393359"/>
+        <c:axId val="68280613"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1325,7 +1325,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49361713"/>
+        <c:crossAx val="31811527"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1661,11 +1661,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="40309888"/>
-        <c:axId val="60067954"/>
+        <c:axId val="59715639"/>
+        <c:axId val="1674237"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="40309888"/>
+        <c:axId val="59715639"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1739,14 +1739,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60067954"/>
+        <c:crossAx val="1674237"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60067954"/>
+        <c:axId val="1674237"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1827,7 +1827,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40309888"/>
+        <c:crossAx val="59715639"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2163,11 +2163,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="64891630"/>
-        <c:axId val="78155265"/>
+        <c:axId val="3716769"/>
+        <c:axId val="91972532"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="64891630"/>
+        <c:axId val="3716769"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2241,14 +2241,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78155265"/>
+        <c:crossAx val="91972532"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78155265"/>
+        <c:axId val="91972532"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2329,7 +2329,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64891630"/>
+        <c:crossAx val="3716769"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2665,11 +2665,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="81186570"/>
-        <c:axId val="38208509"/>
+        <c:axId val="49249998"/>
+        <c:axId val="46725457"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="81186570"/>
+        <c:axId val="49249998"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2743,14 +2743,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38208509"/>
+        <c:crossAx val="46725457"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="38208509"/>
+        <c:axId val="46725457"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2831,7 +2831,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81186570"/>
+        <c:crossAx val="49249998"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3167,11 +3167,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="66886927"/>
-        <c:axId val="69166363"/>
+        <c:axId val="78944110"/>
+        <c:axId val="68732759"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="66886927"/>
+        <c:axId val="78944110"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3245,14 +3245,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69166363"/>
+        <c:crossAx val="68732759"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69166363"/>
+        <c:axId val="68732759"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3333,7 +3333,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66886927"/>
+        <c:crossAx val="78944110"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3610,7 +3610,7 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>6</c:v>
@@ -3628,11 +3628,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="30581476"/>
-        <c:axId val="68919555"/>
+        <c:axId val="98185791"/>
+        <c:axId val="55684900"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="30581476"/>
+        <c:axId val="98185791"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3706,14 +3706,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68919555"/>
+        <c:crossAx val="55684900"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68919555"/>
+        <c:axId val="55684900"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3794,7 +3794,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30581476"/>
+        <c:crossAx val="98185791"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4089,11 +4089,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="81362879"/>
-        <c:axId val="87093365"/>
+        <c:axId val="85884674"/>
+        <c:axId val="88506006"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="81362879"/>
+        <c:axId val="85884674"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4167,14 +4167,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87093365"/>
+        <c:crossAx val="88506006"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87093365"/>
+        <c:axId val="88506006"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4255,7 +4255,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81362879"/>
+        <c:crossAx val="85884674"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4294,9 +4294,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>629640</xdr:colOff>
+      <xdr:colOff>629280</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>22320</xdr:rowOff>
+      <xdr:rowOff>21960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4304,8 +4304,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5819760" y="87480"/>
-        <a:ext cx="12526200" cy="2738880"/>
+        <a:off x="5829120" y="87480"/>
+        <a:ext cx="12592800" cy="2738520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4324,9 +4324,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>203400</xdr:colOff>
+      <xdr:colOff>203040</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>78480</xdr:rowOff>
+      <xdr:rowOff>78120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4334,8 +4334,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5762520" y="80640"/>
-        <a:ext cx="12157200" cy="2626560"/>
+        <a:off x="5771880" y="80640"/>
+        <a:ext cx="12223800" cy="2626200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4359,9 +4359,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>3600</xdr:colOff>
+      <xdr:colOff>3240</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>41760</xdr:rowOff>
+      <xdr:rowOff>41400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4370,7 +4370,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2916360" y="23040"/>
-        <a:ext cx="8002800" cy="2746440"/>
+        <a:ext cx="8049960" cy="2746080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4394,9 +4394,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>331200</xdr:colOff>
+      <xdr:colOff>330840</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>18720</xdr:rowOff>
+      <xdr:rowOff>18360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4405,7 +4405,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5634720" cy="2738880"/>
+        <a:ext cx="5634360" cy="2738520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4429,9 +4429,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>331200</xdr:colOff>
+      <xdr:colOff>330840</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>18720</xdr:rowOff>
+      <xdr:rowOff>18360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4440,7 +4440,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5634720" cy="2738880"/>
+        <a:ext cx="5634360" cy="2738520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4464,9 +4464,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>331200</xdr:colOff>
+      <xdr:colOff>330840</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>18720</xdr:rowOff>
+      <xdr:rowOff>18360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4475,7 +4475,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5634720" cy="2738880"/>
+        <a:ext cx="5634360" cy="2738520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4499,9 +4499,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>331200</xdr:colOff>
+      <xdr:colOff>330840</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>18720</xdr:rowOff>
+      <xdr:rowOff>18360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4510,7 +4510,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="23040"/>
-        <a:ext cx="5634720" cy="2738880"/>
+        <a:ext cx="5634360" cy="2738520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4530,8 +4530,8 @@
   </sheetPr>
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E40" activeCellId="0" sqref="E40"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E41" activeCellId="0" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -4539,10 +4539,10 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.5991902834008"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.3481781376518"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.919028340081"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.7732793522267"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.57085020242915"/>
@@ -4668,14 +4668,14 @@
       </c>
       <c r="B12" s="0" t="n">
         <f aca="false">C11-D12</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C12" s="0" t="n">
         <f aca="false">COUNT(B21:B107)</f>
         <v>28</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E12" s="2" t="n">
         <v>43212</v>
@@ -4694,7 +4694,6 @@
         <v>28</v>
       </c>
       <c r="D13" s="1" t="n">
-        <f aca="false">D12</f>
         <v>22</v>
       </c>
       <c r="E13" s="2" t="n">
@@ -5276,7 +5275,7 @@
         <v>4</v>
       </c>
       <c r="E38" s="11" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F38" s="11" t="s">
         <v>42</v>
@@ -5366,7 +5365,7 @@
         <v>5</v>
       </c>
       <c r="E41" s="14" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F41" s="14" t="s">
         <v>29</v>
@@ -5604,8 +5603,8 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="53.2388663967611"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="53.668016194332"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>